<commit_message>
Ciclo de vida y tabla de recursos
</commit_message>
<xml_diff>
--- a/Documentacion/Proyecto/Tabla de Actividades/Tabla de actividades.xlsx
+++ b/Documentacion/Proyecto/Tabla de Actividades/Tabla de actividades.xlsx
@@ -1026,6 +1026,273 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,273 +1330,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1621,8 +1621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M273"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:H89"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1631,74 +1631,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="21"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="110"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="113"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="113"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="102"/>
+      <c r="C4" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="12" t="s">
+      <c r="D4" s="105"/>
+      <c r="E4" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="12" t="s">
+      <c r="F4" s="105"/>
+      <c r="G4" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="16"/>
+      <c r="H4" s="105"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
+      <c r="A5" s="103"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="107"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="25"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="8" t="s">
         <v>208</v>
       </c>
@@ -1711,8 +1711,8 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
       <c r="G7" s="10"/>
@@ -1723,10 +1723,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="31"/>
+      <c r="D8" s="93"/>
       <c r="E8" s="4" t="s">
         <v>208</v>
       </c>
@@ -1739,8 +1739,8 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
       <c r="G9" s="6"/>
@@ -1751,10 +1751,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="9"/>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="8" t="s">
         <v>208</v>
       </c>
@@ -1767,10 +1767,10 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="34"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="10"/>
       <c r="H11" s="11"/>
     </row>
@@ -1779,15 +1779,15 @@
         <v>11</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="93"/>
       <c r="E12" s="4" t="s">
         <v>208</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="31">
+      <c r="G12" s="93">
         <v>1</v>
       </c>
       <c r="H12" s="5"/>
@@ -1795,11 +1795,11 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
       <c r="E13" s="6"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="32"/>
+      <c r="G13" s="94"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1807,10 +1807,10 @@
         <v>211</v>
       </c>
       <c r="B14" s="9"/>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="50"/>
+      <c r="D14" s="57"/>
       <c r="E14" s="8" t="s">
         <v>208</v>
       </c>
@@ -1821,8 +1821,8 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
       <c r="G15" s="10"/>
@@ -1841,7 +1841,9 @@
         <v>208</v>
       </c>
       <c r="F16" s="5"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1855,40 +1857,42 @@
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="45" t="s">
+      <c r="B18" s="89"/>
+      <c r="C18" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="43" t="s">
+      <c r="D18" s="98"/>
+      <c r="E18" s="88" t="s">
         <v>142</v>
       </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="95">
+        <v>1</v>
+      </c>
+      <c r="H18" s="89"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
+      <c r="A19" s="90"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="91"/>
     </row>
     <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="54"/>
-      <c r="C20" s="55" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="60" t="s">
         <v>256</v>
       </c>
-      <c r="D20" s="56"/>
+      <c r="D20" s="61"/>
       <c r="E20" s="4" t="s">
         <v>208</v>
       </c>
@@ -1897,10 +1901,10 @@
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="58"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="63"/>
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
       <c r="G21" s="6"/>
@@ -1919,20 +1923,20 @@
         <v>16</v>
       </c>
       <c r="F22" s="9"/>
-      <c r="G22" s="39">
+      <c r="G22" s="36">
         <v>1</v>
       </c>
-      <c r="H22" s="40"/>
+      <c r="H22" s="37"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
-      <c r="B23" s="34"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="42"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="39"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -1947,8 +1951,10 @@
         <v>211</v>
       </c>
       <c r="F24" s="5"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="54"/>
+      <c r="G24" s="92">
+        <v>1</v>
+      </c>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
@@ -1957,46 +1963,46 @@
       <c r="D25" s="7"/>
       <c r="E25" s="6"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="54"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="17"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="39" t="s">
+      <c r="B26" s="37"/>
+      <c r="C26" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="40"/>
-      <c r="E26" s="70" t="s">
+      <c r="D26" s="37"/>
+      <c r="E26" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="70"/>
+      <c r="F26" s="86"/>
       <c r="G26" s="8">
         <v>1</v>
       </c>
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="28"/>
+      <c r="D28" s="30"/>
       <c r="E28" s="4" t="s">
         <v>208</v>
       </c>
@@ -2009,34 +2015,36 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="30"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="32"/>
       <c r="E29" s="6"/>
       <c r="F29" s="7"/>
       <c r="G29" s="6"/>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="39" t="s">
+      <c r="B30" s="37"/>
+      <c r="C30" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="40"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F30" s="9"/>
-      <c r="G30" s="8"/>
+      <c r="G30" s="8">
+        <v>1</v>
+      </c>
       <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="42"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="39"/>
       <c r="E31" s="10"/>
       <c r="F31" s="11"/>
       <c r="G31" s="10"/>
@@ -2047,10 +2055,10 @@
         <v>257</v>
       </c>
       <c r="B32" s="5"/>
-      <c r="C32" s="66" t="s">
+      <c r="C32" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="67"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="4" t="s">
         <v>208</v>
       </c>
@@ -2061,8 +2069,8 @@
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="69"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
       <c r="E33" s="6"/>
       <c r="F33" s="7"/>
       <c r="G33" s="6"/>
@@ -2095,58 +2103,58 @@
       <c r="H35" s="11"/>
     </row>
     <row r="36" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="87" t="s">
         <v>213</v>
       </c>
-      <c r="B36" s="64"/>
-      <c r="C36" s="63" t="s">
+      <c r="B36" s="34"/>
+      <c r="C36" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="53" t="s">
+      <c r="D36" s="34"/>
+      <c r="E36" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="F36" s="54"/>
+      <c r="F36" s="17"/>
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="32"/>
       <c r="E37" s="6"/>
       <c r="F37" s="7"/>
       <c r="G37" s="6"/>
       <c r="H37" s="7"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="59" t="s">
+      <c r="A38" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="B38" s="60"/>
-      <c r="C38" s="59" t="s">
+      <c r="B38" s="26"/>
+      <c r="C38" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="60"/>
-      <c r="E38" s="59" t="s">
+      <c r="D38" s="26"/>
+      <c r="E38" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="F38" s="60"/>
-      <c r="G38" s="59">
+      <c r="F38" s="26"/>
+      <c r="G38" s="25">
         <v>1</v>
       </c>
-      <c r="H38" s="60"/>
+      <c r="H38" s="26"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="61"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="62"/>
-      <c r="G39" s="61"/>
-      <c r="H39" s="62"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="28"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
@@ -2175,30 +2183,30 @@
       <c r="H41" s="7"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="59" t="s">
+      <c r="A42" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="B42" s="60"/>
-      <c r="C42" s="59" t="s">
+      <c r="B42" s="26"/>
+      <c r="C42" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="60"/>
-      <c r="E42" s="59" t="s">
+      <c r="D42" s="26"/>
+      <c r="E42" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F42" s="60"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="60"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="26"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="61"/>
-      <c r="B43" s="62"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="62"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="62"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="28"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
@@ -2227,30 +2235,30 @@
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="59" t="s">
+      <c r="A46" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="60"/>
-      <c r="C46" s="59" t="s">
+      <c r="B46" s="26"/>
+      <c r="C46" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D46" s="60"/>
-      <c r="E46" s="59" t="s">
+      <c r="D46" s="26"/>
+      <c r="E46" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="60"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="60"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="26"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="61"/>
-      <c r="B47" s="62"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="62"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="62"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="62"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="28"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
@@ -2279,30 +2287,30 @@
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="59" t="s">
+      <c r="A50" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="B50" s="60"/>
-      <c r="C50" s="59" t="s">
+      <c r="B50" s="26"/>
+      <c r="C50" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="60"/>
-      <c r="E50" s="59" t="s">
+      <c r="D50" s="26"/>
+      <c r="E50" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="F50" s="60"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="60"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="26"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="61"/>
-      <c r="B51" s="62"/>
-      <c r="C51" s="61"/>
-      <c r="D51" s="62"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="62"/>
-      <c r="G51" s="61"/>
-      <c r="H51" s="62"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="28"/>
       <c r="M51" s="2"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -2332,40 +2340,40 @@
       <c r="H53" s="7"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="73" t="s">
+      <c r="A54" s="80" t="s">
         <v>216</v>
       </c>
-      <c r="B54" s="74"/>
-      <c r="C54" s="73" t="s">
+      <c r="B54" s="81"/>
+      <c r="C54" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="D54" s="74"/>
-      <c r="E54" s="59" t="s">
+      <c r="D54" s="81"/>
+      <c r="E54" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="F54" s="60"/>
-      <c r="G54" s="59"/>
-      <c r="H54" s="60"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="26"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="75"/>
-      <c r="B55" s="76"/>
-      <c r="C55" s="75"/>
-      <c r="D55" s="76"/>
-      <c r="E55" s="61"/>
-      <c r="F55" s="62"/>
-      <c r="G55" s="71"/>
-      <c r="H55" s="72"/>
+      <c r="A55" s="82"/>
+      <c r="B55" s="83"/>
+      <c r="C55" s="82"/>
+      <c r="D55" s="83"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="84"/>
+      <c r="H55" s="85"/>
     </row>
     <row r="56" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="27" t="s">
+      <c r="A56" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="28"/>
-      <c r="C56" s="27" t="s">
+      <c r="B56" s="30"/>
+      <c r="C56" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D56" s="28"/>
+      <c r="D56" s="30"/>
       <c r="E56" s="4" t="s">
         <v>208</v>
       </c>
@@ -2374,10 +2382,10 @@
       <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="30"/>
+      <c r="A57" s="31"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="32"/>
       <c r="E57" s="6"/>
       <c r="F57" s="7"/>
       <c r="G57" s="6"/>
@@ -2410,14 +2418,14 @@
       <c r="H59" s="11"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="27" t="s">
+      <c r="A60" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B60" s="28"/>
-      <c r="C60" s="27" t="s">
+      <c r="B60" s="30"/>
+      <c r="C60" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D60" s="28"/>
+      <c r="D60" s="30"/>
       <c r="E60" s="4" t="s">
         <v>208</v>
       </c>
@@ -2426,24 +2434,24 @@
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="29"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="30"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="32"/>
       <c r="E61" s="6"/>
       <c r="F61" s="7"/>
       <c r="G61" s="6"/>
       <c r="H61" s="7"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="39" t="s">
+      <c r="A62" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="B62" s="40"/>
-      <c r="C62" s="39" t="s">
+      <c r="B62" s="37"/>
+      <c r="C62" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D62" s="40"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="8" t="s">
         <v>208</v>
       </c>
@@ -2452,10 +2460,10 @@
       <c r="H62" s="9"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="41"/>
-      <c r="B63" s="42"/>
-      <c r="C63" s="41"/>
-      <c r="D63" s="42"/>
+      <c r="A63" s="38"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="39"/>
       <c r="E63" s="10"/>
       <c r="F63" s="11"/>
       <c r="G63" s="10"/>
@@ -2492,10 +2500,10 @@
         <v>36</v>
       </c>
       <c r="B66" s="9"/>
-      <c r="C66" s="49" t="s">
+      <c r="C66" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="D66" s="50"/>
+      <c r="D66" s="57"/>
       <c r="E66" s="8" t="s">
         <v>218</v>
       </c>
@@ -2506,12 +2514,12 @@
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="11"/>
-      <c r="C67" s="51"/>
-      <c r="D67" s="52"/>
+      <c r="C67" s="58"/>
+      <c r="D67" s="59"/>
       <c r="E67" s="10"/>
       <c r="F67" s="11"/>
-      <c r="G67" s="33"/>
-      <c r="H67" s="34"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="15"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
@@ -2544,10 +2552,10 @@
         <v>53</v>
       </c>
       <c r="B70" s="9"/>
-      <c r="C70" s="77" t="s">
+      <c r="C70" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D70" s="78"/>
+      <c r="D70" s="47"/>
       <c r="E70" s="8" t="s">
         <v>218</v>
       </c>
@@ -2558,8 +2566,8 @@
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="11"/>
-      <c r="C71" s="79"/>
-      <c r="D71" s="80"/>
+      <c r="C71" s="48"/>
+      <c r="D71" s="49"/>
       <c r="E71" s="10"/>
       <c r="F71" s="11"/>
       <c r="G71" s="10"/>
@@ -2592,14 +2600,14 @@
       <c r="H73" s="7"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="39" t="s">
+      <c r="A74" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="B74" s="40"/>
-      <c r="C74" s="39" t="s">
+      <c r="B74" s="37"/>
+      <c r="C74" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D74" s="40"/>
+      <c r="D74" s="37"/>
       <c r="E74" s="8" t="s">
         <v>208</v>
       </c>
@@ -2608,10 +2616,10 @@
       <c r="H74" s="9"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="41"/>
-      <c r="B75" s="42"/>
-      <c r="C75" s="41"/>
-      <c r="D75" s="42"/>
+      <c r="A75" s="38"/>
+      <c r="B75" s="39"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="39"/>
       <c r="E75" s="10"/>
       <c r="F75" s="11"/>
       <c r="G75" s="10"/>
@@ -2622,10 +2630,10 @@
         <v>219</v>
       </c>
       <c r="B76" s="5"/>
-      <c r="C76" s="55" t="s">
+      <c r="C76" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="D76" s="56"/>
+      <c r="D76" s="61"/>
       <c r="E76" s="4" t="s">
         <v>208</v>
       </c>
@@ -2636,22 +2644,22 @@
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="7"/>
-      <c r="C77" s="57"/>
-      <c r="D77" s="58"/>
+      <c r="C77" s="62"/>
+      <c r="D77" s="63"/>
       <c r="E77" s="6"/>
       <c r="F77" s="7"/>
       <c r="G77" s="6"/>
       <c r="H77" s="7"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="39" t="s">
+      <c r="A78" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="B78" s="40"/>
-      <c r="C78" s="73" t="s">
+      <c r="B78" s="37"/>
+      <c r="C78" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="D78" s="74"/>
+      <c r="D78" s="81"/>
       <c r="E78" s="8" t="s">
         <v>208</v>
       </c>
@@ -2660,10 +2668,10 @@
       <c r="H78" s="9"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="41"/>
-      <c r="B79" s="42"/>
-      <c r="C79" s="75"/>
-      <c r="D79" s="76"/>
+      <c r="A79" s="38"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="82"/>
+      <c r="D79" s="83"/>
       <c r="E79" s="10"/>
       <c r="F79" s="11"/>
       <c r="G79" s="10"/>
@@ -2726,10 +2734,10 @@
         <v>154</v>
       </c>
       <c r="B84" s="5"/>
-      <c r="C84" s="85" t="s">
+      <c r="C84" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="D84" s="86"/>
+      <c r="D84" s="65"/>
       <c r="E84" s="4" t="s">
         <v>208</v>
       </c>
@@ -2740,8 +2748,8 @@
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="7"/>
-      <c r="C85" s="87"/>
-      <c r="D85" s="88"/>
+      <c r="C85" s="66"/>
+      <c r="D85" s="67"/>
       <c r="E85" s="6"/>
       <c r="F85" s="7"/>
       <c r="G85" s="6"/>
@@ -2752,10 +2760,10 @@
         <v>155</v>
       </c>
       <c r="B86" s="9"/>
-      <c r="C86" s="81" t="s">
+      <c r="C86" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="D86" s="82"/>
+      <c r="D86" s="77"/>
       <c r="E86" s="8" t="s">
         <v>208</v>
       </c>
@@ -2766,34 +2774,34 @@
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="10"/>
       <c r="B87" s="11"/>
-      <c r="C87" s="83"/>
-      <c r="D87" s="84"/>
+      <c r="C87" s="78"/>
+      <c r="D87" s="79"/>
       <c r="E87" s="10"/>
       <c r="F87" s="11"/>
       <c r="G87" s="10"/>
       <c r="H87" s="11"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="111" t="s">
+      <c r="A88" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B88" s="112"/>
-      <c r="C88" s="112"/>
-      <c r="D88" s="112"/>
-      <c r="E88" s="112"/>
-      <c r="F88" s="112"/>
-      <c r="G88" s="112"/>
-      <c r="H88" s="113"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="19"/>
+      <c r="H88" s="20"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="111"/>
-      <c r="B89" s="112"/>
-      <c r="C89" s="112"/>
-      <c r="D89" s="112"/>
-      <c r="E89" s="112"/>
-      <c r="F89" s="112"/>
-      <c r="G89" s="112"/>
-      <c r="H89" s="113"/>
+      <c r="A89" s="18"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="20"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
@@ -2824,10 +2832,10 @@
         <v>222</v>
       </c>
       <c r="B92" s="5"/>
-      <c r="C92" s="89" t="s">
+      <c r="C92" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="D92" s="90"/>
+      <c r="D92" s="73"/>
       <c r="E92" s="4"/>
       <c r="F92" s="5"/>
       <c r="G92" s="4"/>
@@ -2836,8 +2844,8 @@
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="7"/>
-      <c r="C93" s="91"/>
-      <c r="D93" s="92"/>
+      <c r="C93" s="74"/>
+      <c r="D93" s="75"/>
       <c r="E93" s="6"/>
       <c r="F93" s="7"/>
       <c r="G93" s="6"/>
@@ -2868,18 +2876,18 @@
       <c r="H95" s="11"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="53" t="s">
+      <c r="A96" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="B96" s="54"/>
+      <c r="B96" s="17"/>
       <c r="C96" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D96" s="5"/>
       <c r="E96" s="4"/>
       <c r="F96" s="5"/>
-      <c r="G96" s="53"/>
-      <c r="H96" s="54"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="17"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
@@ -2964,14 +2972,14 @@
       <c r="H103" s="11"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="53" t="s">
+      <c r="A104" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="B104" s="54"/>
-      <c r="C104" s="55" t="s">
+      <c r="B104" s="17"/>
+      <c r="C104" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="D104" s="56"/>
+      <c r="D104" s="61"/>
       <c r="E104" s="4"/>
       <c r="F104" s="5"/>
       <c r="G104" s="4"/>
@@ -2980,8 +2988,8 @@
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="7"/>
-      <c r="C105" s="57"/>
-      <c r="D105" s="58"/>
+      <c r="C105" s="62"/>
+      <c r="D105" s="63"/>
       <c r="E105" s="6"/>
       <c r="F105" s="7"/>
       <c r="G105" s="6"/>
@@ -3054,8 +3062,8 @@
       <c r="B111" s="11"/>
       <c r="C111" s="10"/>
       <c r="D111" s="11"/>
-      <c r="E111" s="33"/>
-      <c r="F111" s="34"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="15"/>
       <c r="G111" s="10"/>
       <c r="H111" s="11"/>
     </row>
@@ -3116,8 +3124,8 @@
         <v>73</v>
       </c>
       <c r="D116" s="5"/>
-      <c r="E116" s="53"/>
-      <c r="F116" s="54"/>
+      <c r="E116" s="16"/>
+      <c r="F116" s="17"/>
       <c r="G116" s="4"/>
       <c r="H116" s="5"/>
     </row>
@@ -3132,22 +3140,22 @@
       <c r="H117" s="7"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="33" t="s">
+      <c r="A118" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="B118" s="34"/>
-      <c r="C118" s="33" t="s">
+      <c r="B118" s="15"/>
+      <c r="C118" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D118" s="34"/>
-      <c r="E118" s="33"/>
-      <c r="F118" s="34"/>
-      <c r="G118" s="33"/>
-      <c r="H118" s="34"/>
+      <c r="D118" s="15"/>
+      <c r="E118" s="14"/>
+      <c r="F118" s="15"/>
+      <c r="G118" s="14"/>
+      <c r="H118" s="15"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="33"/>
-      <c r="B119" s="34"/>
+      <c r="A119" s="14"/>
+      <c r="B119" s="15"/>
       <c r="C119" s="10"/>
       <c r="D119" s="11"/>
       <c r="E119" s="10"/>
@@ -3160,10 +3168,10 @@
         <v>226</v>
       </c>
       <c r="B120" s="5"/>
-      <c r="C120" s="55" t="s">
+      <c r="C120" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="D120" s="56"/>
+      <c r="D120" s="61"/>
       <c r="E120" s="4"/>
       <c r="F120" s="5"/>
       <c r="G120" s="4"/>
@@ -3172,8 +3180,8 @@
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="6"/>
       <c r="B121" s="7"/>
-      <c r="C121" s="57"/>
-      <c r="D121" s="58"/>
+      <c r="C121" s="62"/>
+      <c r="D121" s="63"/>
       <c r="E121" s="6"/>
       <c r="F121" s="7"/>
       <c r="G121" s="6"/>
@@ -3204,10 +3212,10 @@
       <c r="H123" s="11"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="53" t="s">
+      <c r="A124" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="B124" s="54"/>
+      <c r="B124" s="17"/>
       <c r="C124" s="4" t="s">
         <v>77</v>
       </c>
@@ -3232,10 +3240,10 @@
         <v>167</v>
       </c>
       <c r="B126" s="9"/>
-      <c r="C126" s="49" t="s">
+      <c r="C126" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="D126" s="50"/>
+      <c r="D126" s="57"/>
       <c r="E126" s="8"/>
       <c r="F126" s="9"/>
       <c r="G126" s="8"/>
@@ -3244,8 +3252,8 @@
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="10"/>
       <c r="B127" s="11"/>
-      <c r="C127" s="51"/>
-      <c r="D127" s="52"/>
+      <c r="C127" s="58"/>
+      <c r="D127" s="59"/>
       <c r="E127" s="10"/>
       <c r="F127" s="11"/>
       <c r="G127" s="10"/>
@@ -3304,10 +3312,10 @@
         <v>170</v>
       </c>
       <c r="B132" s="5"/>
-      <c r="C132" s="66" t="s">
+      <c r="C132" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D132" s="67"/>
+      <c r="D132" s="22"/>
       <c r="E132" s="4"/>
       <c r="F132" s="5"/>
       <c r="G132" s="4"/>
@@ -3316,8 +3324,8 @@
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="6"/>
       <c r="B133" s="7"/>
-      <c r="C133" s="68"/>
-      <c r="D133" s="69"/>
+      <c r="C133" s="23"/>
+      <c r="D133" s="24"/>
       <c r="E133" s="6"/>
       <c r="F133" s="7"/>
       <c r="G133" s="6"/>
@@ -3352,10 +3360,10 @@
         <v>228</v>
       </c>
       <c r="B136" s="5"/>
-      <c r="C136" s="55" t="s">
+      <c r="C136" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="D136" s="93"/>
+      <c r="D136" s="70"/>
       <c r="E136" s="4"/>
       <c r="F136" s="5"/>
       <c r="G136" s="4"/>
@@ -3364,8 +3372,8 @@
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="6"/>
       <c r="B137" s="7"/>
-      <c r="C137" s="57"/>
-      <c r="D137" s="94"/>
+      <c r="C137" s="62"/>
+      <c r="D137" s="71"/>
       <c r="E137" s="6"/>
       <c r="F137" s="7"/>
       <c r="G137" s="6"/>
@@ -3388,8 +3396,8 @@
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="10"/>
       <c r="B139" s="11"/>
-      <c r="C139" s="33"/>
-      <c r="D139" s="34"/>
+      <c r="C139" s="14"/>
+      <c r="D139" s="15"/>
       <c r="E139" s="10"/>
       <c r="F139" s="11"/>
       <c r="G139" s="10"/>
@@ -3451,10 +3459,10 @@
         <v>231</v>
       </c>
       <c r="B144" s="5"/>
-      <c r="C144" s="53" t="s">
+      <c r="C144" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D144" s="54"/>
+      <c r="D144" s="17"/>
       <c r="E144" s="4"/>
       <c r="F144" s="5"/>
       <c r="G144" s="4"/>
@@ -3499,10 +3507,10 @@
         <v>233</v>
       </c>
       <c r="B148" s="5"/>
-      <c r="C148" s="66" t="s">
+      <c r="C148" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D148" s="67"/>
+      <c r="D148" s="22"/>
       <c r="E148" s="4"/>
       <c r="F148" s="5"/>
       <c r="G148" s="4"/>
@@ -3511,8 +3519,8 @@
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="6"/>
       <c r="B149" s="7"/>
-      <c r="C149" s="68"/>
-      <c r="D149" s="69"/>
+      <c r="C149" s="23"/>
+      <c r="D149" s="24"/>
       <c r="E149" s="6"/>
       <c r="F149" s="7"/>
       <c r="G149" s="6"/>
@@ -3524,10 +3532,10 @@
         <v>234</v>
       </c>
       <c r="B150" s="9"/>
-      <c r="C150" s="49" t="s">
+      <c r="C150" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="D150" s="50"/>
+      <c r="D150" s="57"/>
       <c r="E150" s="8"/>
       <c r="F150" s="9"/>
       <c r="G150" s="8"/>
@@ -3536,8 +3544,8 @@
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="10"/>
       <c r="B151" s="11"/>
-      <c r="C151" s="51"/>
-      <c r="D151" s="52"/>
+      <c r="C151" s="58"/>
+      <c r="D151" s="59"/>
       <c r="E151" s="10"/>
       <c r="F151" s="11"/>
       <c r="G151" s="10"/>
@@ -3620,10 +3628,10 @@
         <v>236</v>
       </c>
       <c r="B158" s="9"/>
-      <c r="C158" s="49" t="s">
+      <c r="C158" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="D158" s="50"/>
+      <c r="D158" s="57"/>
       <c r="E158" s="8"/>
       <c r="F158" s="9"/>
       <c r="G158" s="8"/>
@@ -3632,8 +3640,8 @@
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="10"/>
       <c r="B159" s="11"/>
-      <c r="C159" s="95"/>
-      <c r="D159" s="96"/>
+      <c r="C159" s="68"/>
+      <c r="D159" s="69"/>
       <c r="E159" s="10"/>
       <c r="F159" s="11"/>
       <c r="G159" s="10"/>
@@ -3667,35 +3675,35 @@
       <c r="A162" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B162" s="25"/>
+      <c r="B162" s="12"/>
       <c r="C162" s="8" t="s">
         <v>96</v>
       </c>
       <c r="D162" s="9"/>
       <c r="E162" s="8"/>
       <c r="F162" s="9"/>
-      <c r="G162" s="25"/>
+      <c r="G162" s="12"/>
       <c r="H162" s="9"/>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="10"/>
-      <c r="B163" s="26"/>
+      <c r="B163" s="13"/>
       <c r="C163" s="10"/>
       <c r="D163" s="11"/>
       <c r="E163" s="10"/>
       <c r="F163" s="11"/>
-      <c r="G163" s="26"/>
+      <c r="G163" s="13"/>
       <c r="H163" s="11"/>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A164" s="53" t="s">
+      <c r="A164" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="B164" s="54"/>
-      <c r="C164" s="66" t="s">
+      <c r="B164" s="17"/>
+      <c r="C164" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="D164" s="67"/>
+      <c r="D164" s="22"/>
       <c r="E164" s="4"/>
       <c r="F164" s="5"/>
       <c r="G164" s="4"/>
@@ -3704,8 +3712,8 @@
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="6"/>
       <c r="B165" s="7"/>
-      <c r="C165" s="68"/>
-      <c r="D165" s="69"/>
+      <c r="C165" s="23"/>
+      <c r="D165" s="24"/>
       <c r="E165" s="6"/>
       <c r="F165" s="7"/>
       <c r="G165" s="6"/>
@@ -3716,10 +3724,10 @@
         <v>177</v>
       </c>
       <c r="B166" s="9"/>
-      <c r="C166" s="49" t="s">
+      <c r="C166" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="D166" s="50"/>
+      <c r="D166" s="57"/>
       <c r="E166" s="8"/>
       <c r="F166" s="9"/>
       <c r="G166" s="8"/>
@@ -3728,8 +3736,8 @@
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="10"/>
       <c r="B167" s="11"/>
-      <c r="C167" s="51"/>
-      <c r="D167" s="52"/>
+      <c r="C167" s="58"/>
+      <c r="D167" s="59"/>
       <c r="E167" s="10"/>
       <c r="F167" s="11"/>
       <c r="G167" s="10"/>
@@ -3740,10 +3748,10 @@
         <v>178</v>
       </c>
       <c r="B168" s="5"/>
-      <c r="C168" s="66" t="s">
+      <c r="C168" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D168" s="67"/>
+      <c r="D168" s="22"/>
       <c r="E168" s="4"/>
       <c r="F168" s="5"/>
       <c r="G168" s="4"/>
@@ -3752,8 +3760,8 @@
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="6"/>
       <c r="B169" s="7"/>
-      <c r="C169" s="68"/>
-      <c r="D169" s="69"/>
+      <c r="C169" s="23"/>
+      <c r="D169" s="24"/>
       <c r="E169" s="6"/>
       <c r="F169" s="7"/>
       <c r="G169" s="6"/>
@@ -3788,10 +3796,10 @@
         <v>239</v>
       </c>
       <c r="B172" s="5"/>
-      <c r="C172" s="85" t="s">
+      <c r="C172" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="D172" s="86"/>
+      <c r="D172" s="65"/>
       <c r="E172" s="4"/>
       <c r="F172" s="5"/>
       <c r="G172" s="4"/>
@@ -3800,8 +3808,8 @@
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="6"/>
       <c r="B173" s="7"/>
-      <c r="C173" s="87"/>
-      <c r="D173" s="88"/>
+      <c r="C173" s="66"/>
+      <c r="D173" s="67"/>
       <c r="E173" s="6"/>
       <c r="F173" s="7"/>
       <c r="G173" s="6"/>
@@ -3812,10 +3820,10 @@
         <v>179</v>
       </c>
       <c r="B174" s="9"/>
-      <c r="C174" s="77" t="s">
+      <c r="C174" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="D174" s="78"/>
+      <c r="D174" s="47"/>
       <c r="E174" s="8"/>
       <c r="F174" s="9"/>
       <c r="G174" s="8"/>
@@ -3824,8 +3832,8 @@
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="10"/>
       <c r="B175" s="11"/>
-      <c r="C175" s="79"/>
-      <c r="D175" s="80"/>
+      <c r="C175" s="48"/>
+      <c r="D175" s="49"/>
       <c r="E175" s="10"/>
       <c r="F175" s="11"/>
       <c r="G175" s="10"/>
@@ -3884,10 +3892,10 @@
         <v>182</v>
       </c>
       <c r="B180" s="5"/>
-      <c r="C180" s="66" t="s">
+      <c r="C180" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D180" s="67"/>
+      <c r="D180" s="22"/>
       <c r="E180" s="4"/>
       <c r="F180" s="5"/>
       <c r="G180" s="4"/>
@@ -3896,8 +3904,8 @@
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="6"/>
       <c r="B181" s="7"/>
-      <c r="C181" s="68"/>
-      <c r="D181" s="69"/>
+      <c r="C181" s="23"/>
+      <c r="D181" s="24"/>
       <c r="E181" s="6"/>
       <c r="F181" s="7"/>
       <c r="G181" s="6"/>
@@ -3928,26 +3936,26 @@
       <c r="H183" s="11"/>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A184" s="111" t="s">
+      <c r="A184" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B184" s="112"/>
-      <c r="C184" s="112"/>
-      <c r="D184" s="112"/>
-      <c r="E184" s="112"/>
-      <c r="F184" s="112"/>
-      <c r="G184" s="112"/>
-      <c r="H184" s="113"/>
+      <c r="B184" s="19"/>
+      <c r="C184" s="19"/>
+      <c r="D184" s="19"/>
+      <c r="E184" s="19"/>
+      <c r="F184" s="19"/>
+      <c r="G184" s="19"/>
+      <c r="H184" s="20"/>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A185" s="111"/>
-      <c r="B185" s="112"/>
-      <c r="C185" s="112"/>
-      <c r="D185" s="112"/>
-      <c r="E185" s="112"/>
-      <c r="F185" s="112"/>
-      <c r="G185" s="112"/>
-      <c r="H185" s="113"/>
+      <c r="A185" s="18"/>
+      <c r="B185" s="19"/>
+      <c r="C185" s="19"/>
+      <c r="D185" s="19"/>
+      <c r="E185" s="19"/>
+      <c r="F185" s="19"/>
+      <c r="G185" s="19"/>
+      <c r="H185" s="20"/>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="8" t="s">
@@ -3978,10 +3986,10 @@
         <v>241</v>
       </c>
       <c r="B188" s="5"/>
-      <c r="C188" s="55" t="s">
+      <c r="C188" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="D188" s="56"/>
+      <c r="D188" s="61"/>
       <c r="E188" s="4"/>
       <c r="F188" s="5"/>
       <c r="G188" s="4"/>
@@ -3990,8 +3998,8 @@
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="6"/>
       <c r="B189" s="7"/>
-      <c r="C189" s="57"/>
-      <c r="D189" s="58"/>
+      <c r="C189" s="62"/>
+      <c r="D189" s="63"/>
       <c r="E189" s="6"/>
       <c r="F189" s="7"/>
       <c r="G189" s="6"/>
@@ -4050,10 +4058,10 @@
         <v>186</v>
       </c>
       <c r="B194" s="9"/>
-      <c r="C194" s="49" t="s">
+      <c r="C194" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="D194" s="50"/>
+      <c r="D194" s="57"/>
       <c r="E194" s="8"/>
       <c r="F194" s="9"/>
       <c r="G194" s="8"/>
@@ -4062,8 +4070,8 @@
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="10"/>
       <c r="B195" s="11"/>
-      <c r="C195" s="51"/>
-      <c r="D195" s="52"/>
+      <c r="C195" s="58"/>
+      <c r="D195" s="59"/>
       <c r="E195" s="10"/>
       <c r="F195" s="11"/>
       <c r="G195" s="10"/>
@@ -4074,10 +4082,10 @@
         <v>187</v>
       </c>
       <c r="B196" s="5"/>
-      <c r="C196" s="55" t="s">
+      <c r="C196" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="D196" s="56"/>
+      <c r="D196" s="61"/>
       <c r="E196" s="4"/>
       <c r="F196" s="5"/>
       <c r="G196" s="4"/>
@@ -4086,8 +4094,8 @@
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="6"/>
       <c r="B197" s="7"/>
-      <c r="C197" s="57"/>
-      <c r="D197" s="58"/>
+      <c r="C197" s="62"/>
+      <c r="D197" s="63"/>
       <c r="E197" s="6"/>
       <c r="F197" s="7"/>
       <c r="G197" s="6"/>
@@ -4122,10 +4130,10 @@
         <v>243</v>
       </c>
       <c r="B200" s="5"/>
-      <c r="C200" s="66" t="s">
+      <c r="C200" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D200" s="67"/>
+      <c r="D200" s="22"/>
       <c r="E200" s="4"/>
       <c r="F200" s="5"/>
       <c r="G200" s="4"/>
@@ -4134,8 +4142,8 @@
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="6"/>
       <c r="B201" s="7"/>
-      <c r="C201" s="68"/>
-      <c r="D201" s="69"/>
+      <c r="C201" s="23"/>
+      <c r="D201" s="24"/>
       <c r="E201" s="6"/>
       <c r="F201" s="7"/>
       <c r="G201" s="6"/>
@@ -4146,10 +4154,10 @@
         <v>188</v>
       </c>
       <c r="B202" s="9"/>
-      <c r="C202" s="49" t="s">
+      <c r="C202" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="D202" s="50"/>
+      <c r="D202" s="57"/>
       <c r="E202" s="8"/>
       <c r="F202" s="9"/>
       <c r="G202" s="8"/>
@@ -4158,8 +4166,8 @@
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="10"/>
       <c r="B203" s="11"/>
-      <c r="C203" s="51"/>
-      <c r="D203" s="52"/>
+      <c r="C203" s="58"/>
+      <c r="D203" s="59"/>
       <c r="E203" s="10"/>
       <c r="F203" s="11"/>
       <c r="G203" s="10"/>
@@ -4195,10 +4203,10 @@
         <v>190</v>
       </c>
       <c r="B206" s="9"/>
-      <c r="C206" s="49" t="s">
+      <c r="C206" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="D206" s="50"/>
+      <c r="D206" s="57"/>
       <c r="E206" s="8"/>
       <c r="F206" s="9"/>
       <c r="G206" s="8"/>
@@ -4207,8 +4215,8 @@
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="10"/>
       <c r="B207" s="11"/>
-      <c r="C207" s="51"/>
-      <c r="D207" s="52"/>
+      <c r="C207" s="58"/>
+      <c r="D207" s="59"/>
       <c r="E207" s="10"/>
       <c r="F207" s="11"/>
       <c r="G207" s="10"/>
@@ -4264,14 +4272,14 @@
       <c r="H211" s="11"/>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A212" s="53" t="s">
+      <c r="A212" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="B212" s="54"/>
-      <c r="C212" s="66" t="s">
+      <c r="B212" s="17"/>
+      <c r="C212" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="D212" s="67"/>
+      <c r="D212" s="22"/>
       <c r="E212" s="4"/>
       <c r="F212" s="5"/>
       <c r="G212" s="4"/>
@@ -4280,8 +4288,8 @@
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="6"/>
       <c r="B213" s="7"/>
-      <c r="C213" s="68"/>
-      <c r="D213" s="69"/>
+      <c r="C213" s="23"/>
+      <c r="D213" s="24"/>
       <c r="E213" s="6"/>
       <c r="F213" s="7"/>
       <c r="G213" s="6"/>
@@ -4436,10 +4444,10 @@
         <v>195</v>
       </c>
       <c r="B226" s="9"/>
-      <c r="C226" s="77" t="s">
+      <c r="C226" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="D226" s="78"/>
+      <c r="D226" s="47"/>
       <c r="E226" s="8"/>
       <c r="F226" s="9"/>
       <c r="G226" s="8"/>
@@ -4448,32 +4456,32 @@
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="10"/>
       <c r="B227" s="11"/>
-      <c r="C227" s="79"/>
-      <c r="D227" s="80"/>
+      <c r="C227" s="48"/>
+      <c r="D227" s="49"/>
       <c r="E227" s="10"/>
       <c r="F227" s="11"/>
       <c r="G227" s="10"/>
       <c r="H227" s="11"/>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A228" s="53" t="s">
+      <c r="A228" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="B228" s="54"/>
-      <c r="C228" s="97" t="s">
+      <c r="B228" s="17"/>
+      <c r="C228" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="D228" s="98"/>
-      <c r="E228" s="53"/>
-      <c r="F228" s="54"/>
-      <c r="G228" s="53"/>
-      <c r="H228" s="54"/>
+      <c r="D228" s="55"/>
+      <c r="E228" s="16"/>
+      <c r="F228" s="17"/>
+      <c r="G228" s="16"/>
+      <c r="H228" s="17"/>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="6"/>
       <c r="B229" s="7"/>
-      <c r="C229" s="97"/>
-      <c r="D229" s="98"/>
+      <c r="C229" s="54"/>
+      <c r="D229" s="55"/>
       <c r="E229" s="6"/>
       <c r="F229" s="7"/>
       <c r="G229" s="6"/>
@@ -4483,22 +4491,22 @@
       <c r="A230" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="B230" s="25"/>
+      <c r="B230" s="12"/>
       <c r="C230" s="8" t="s">
         <v>124</v>
       </c>
       <c r="D230" s="9"/>
-      <c r="E230" s="25"/>
+      <c r="E230" s="12"/>
       <c r="F230" s="9"/>
       <c r="G230" s="8"/>
       <c r="H230" s="9"/>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="10"/>
-      <c r="B231" s="26"/>
+      <c r="B231" s="13"/>
       <c r="C231" s="10"/>
       <c r="D231" s="11"/>
-      <c r="E231" s="26"/>
+      <c r="E231" s="13"/>
       <c r="F231" s="11"/>
       <c r="G231" s="10"/>
       <c r="H231" s="11"/>
@@ -4508,10 +4516,10 @@
         <v>249</v>
       </c>
       <c r="B232" s="5"/>
-      <c r="C232" s="53" t="s">
+      <c r="C232" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="D232" s="54"/>
+      <c r="D232" s="17"/>
       <c r="E232" s="4"/>
       <c r="F232" s="5"/>
       <c r="G232" s="4"/>
@@ -4576,38 +4584,38 @@
       <c r="H237" s="7"/>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A238" s="59" t="s">
+      <c r="A238" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="B238" s="60"/>
-      <c r="C238" s="59" t="s">
+      <c r="B238" s="26"/>
+      <c r="C238" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D238" s="60"/>
-      <c r="E238" s="59"/>
-      <c r="F238" s="60"/>
-      <c r="G238" s="59"/>
-      <c r="H238" s="60"/>
+      <c r="D238" s="26"/>
+      <c r="E238" s="25"/>
+      <c r="F238" s="26"/>
+      <c r="G238" s="25"/>
+      <c r="H238" s="26"/>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A239" s="61"/>
-      <c r="B239" s="62"/>
-      <c r="C239" s="61"/>
-      <c r="D239" s="62"/>
-      <c r="E239" s="61"/>
-      <c r="F239" s="62"/>
-      <c r="G239" s="61"/>
-      <c r="H239" s="62"/>
+      <c r="A239" s="27"/>
+      <c r="B239" s="28"/>
+      <c r="C239" s="27"/>
+      <c r="D239" s="28"/>
+      <c r="E239" s="27"/>
+      <c r="F239" s="28"/>
+      <c r="G239" s="27"/>
+      <c r="H239" s="28"/>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="4" t="s">
         <v>200</v>
       </c>
       <c r="B240" s="5"/>
-      <c r="C240" s="66" t="s">
+      <c r="C240" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="D240" s="67"/>
+      <c r="D240" s="22"/>
       <c r="E240" s="4"/>
       <c r="F240" s="5"/>
       <c r="G240" s="4"/>
@@ -4616,8 +4624,8 @@
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="6"/>
       <c r="B241" s="7"/>
-      <c r="C241" s="68"/>
-      <c r="D241" s="69"/>
+      <c r="C241" s="23"/>
+      <c r="D241" s="24"/>
       <c r="E241" s="6"/>
       <c r="F241" s="7"/>
       <c r="G241" s="6"/>
@@ -4652,10 +4660,10 @@
         <v>251</v>
       </c>
       <c r="B244" s="5"/>
-      <c r="C244" s="66" t="s">
+      <c r="C244" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="D244" s="67"/>
+      <c r="D244" s="22"/>
       <c r="E244" s="4"/>
       <c r="F244" s="5"/>
       <c r="G244" s="4"/>
@@ -4664,8 +4672,8 @@
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="6"/>
       <c r="B245" s="7"/>
-      <c r="C245" s="68"/>
-      <c r="D245" s="69"/>
+      <c r="C245" s="23"/>
+      <c r="D245" s="24"/>
       <c r="E245" s="6"/>
       <c r="F245" s="7"/>
       <c r="G245" s="6"/>
@@ -4676,10 +4684,10 @@
         <v>252</v>
       </c>
       <c r="B246" s="9"/>
-      <c r="C246" s="77" t="s">
+      <c r="C246" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="D246" s="78"/>
+      <c r="D246" s="47"/>
       <c r="E246" s="8"/>
       <c r="F246" s="9"/>
       <c r="G246" s="8"/>
@@ -4688,8 +4696,8 @@
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="10"/>
       <c r="B247" s="11"/>
-      <c r="C247" s="79"/>
-      <c r="D247" s="80"/>
+      <c r="C247" s="48"/>
+      <c r="D247" s="49"/>
       <c r="E247" s="10"/>
       <c r="F247" s="11"/>
       <c r="G247" s="10"/>
@@ -4704,44 +4712,44 @@
         <v>133</v>
       </c>
       <c r="D248" s="5"/>
-      <c r="E248" s="27"/>
-      <c r="F248" s="28"/>
-      <c r="G248" s="107"/>
-      <c r="H248" s="64"/>
+      <c r="E248" s="29"/>
+      <c r="F248" s="30"/>
+      <c r="G248" s="33"/>
+      <c r="H248" s="34"/>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="6"/>
       <c r="B249" s="7"/>
       <c r="C249" s="6"/>
       <c r="D249" s="7"/>
-      <c r="E249" s="29"/>
-      <c r="F249" s="30"/>
-      <c r="G249" s="108"/>
-      <c r="H249" s="30"/>
+      <c r="E249" s="31"/>
+      <c r="F249" s="32"/>
+      <c r="G249" s="35"/>
+      <c r="H249" s="32"/>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A250" s="33" t="s">
+      <c r="A250" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="B250" s="34"/>
-      <c r="C250" s="33" t="s">
+      <c r="B250" s="15"/>
+      <c r="C250" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D250" s="34"/>
-      <c r="E250" s="109"/>
-      <c r="F250" s="110"/>
-      <c r="G250" s="109"/>
-      <c r="H250" s="110"/>
+      <c r="D250" s="15"/>
+      <c r="E250" s="40"/>
+      <c r="F250" s="41"/>
+      <c r="G250" s="40"/>
+      <c r="H250" s="41"/>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="10"/>
       <c r="B251" s="11"/>
       <c r="C251" s="10"/>
       <c r="D251" s="11"/>
-      <c r="E251" s="41"/>
-      <c r="F251" s="42"/>
-      <c r="G251" s="41"/>
-      <c r="H251" s="42"/>
+      <c r="E251" s="38"/>
+      <c r="F251" s="39"/>
+      <c r="G251" s="38"/>
+      <c r="H251" s="39"/>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="4" t="s">
@@ -4752,20 +4760,20 @@
         <v>135</v>
       </c>
       <c r="D252" s="5"/>
-      <c r="E252" s="27"/>
-      <c r="F252" s="28"/>
-      <c r="G252" s="27"/>
-      <c r="H252" s="28"/>
+      <c r="E252" s="29"/>
+      <c r="F252" s="30"/>
+      <c r="G252" s="29"/>
+      <c r="H252" s="30"/>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="6"/>
       <c r="B253" s="7"/>
       <c r="C253" s="6"/>
       <c r="D253" s="7"/>
-      <c r="E253" s="29"/>
-      <c r="F253" s="30"/>
-      <c r="G253" s="29"/>
-      <c r="H253" s="30"/>
+      <c r="E253" s="31"/>
+      <c r="F253" s="32"/>
+      <c r="G253" s="31"/>
+      <c r="H253" s="32"/>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="8" t="s">
@@ -4776,20 +4784,20 @@
         <v>136</v>
       </c>
       <c r="D254" s="9"/>
-      <c r="E254" s="39"/>
-      <c r="F254" s="40"/>
-      <c r="G254" s="39"/>
-      <c r="H254" s="40"/>
+      <c r="E254" s="36"/>
+      <c r="F254" s="37"/>
+      <c r="G254" s="36"/>
+      <c r="H254" s="37"/>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="10"/>
       <c r="B255" s="11"/>
       <c r="C255" s="10"/>
       <c r="D255" s="11"/>
-      <c r="E255" s="41"/>
-      <c r="F255" s="42"/>
-      <c r="G255" s="41"/>
-      <c r="H255" s="42"/>
+      <c r="E255" s="38"/>
+      <c r="F255" s="39"/>
+      <c r="G255" s="38"/>
+      <c r="H255" s="39"/>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="4" t="s">
@@ -4800,553 +4808,188 @@
         <v>137</v>
       </c>
       <c r="D256" s="5"/>
-      <c r="E256" s="27"/>
-      <c r="F256" s="28"/>
-      <c r="G256" s="27"/>
-      <c r="H256" s="28"/>
+      <c r="E256" s="29"/>
+      <c r="F256" s="30"/>
+      <c r="G256" s="29"/>
+      <c r="H256" s="30"/>
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="6"/>
       <c r="B257" s="7"/>
       <c r="C257" s="6"/>
       <c r="D257" s="7"/>
-      <c r="E257" s="29"/>
-      <c r="F257" s="30"/>
-      <c r="G257" s="29"/>
-      <c r="H257" s="30"/>
+      <c r="E257" s="31"/>
+      <c r="F257" s="32"/>
+      <c r="G257" s="31"/>
+      <c r="H257" s="32"/>
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="8" t="s">
         <v>254</v>
       </c>
       <c r="B258" s="9"/>
-      <c r="C258" s="77" t="s">
+      <c r="C258" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="D258" s="78"/>
-      <c r="E258" s="39"/>
-      <c r="F258" s="40"/>
-      <c r="G258" s="39"/>
-      <c r="H258" s="40"/>
+      <c r="D258" s="47"/>
+      <c r="E258" s="36"/>
+      <c r="F258" s="37"/>
+      <c r="G258" s="36"/>
+      <c r="H258" s="37"/>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="10"/>
       <c r="B259" s="11"/>
-      <c r="C259" s="79"/>
-      <c r="D259" s="80"/>
-      <c r="E259" s="41"/>
-      <c r="F259" s="42"/>
-      <c r="G259" s="41"/>
-      <c r="H259" s="42"/>
+      <c r="C259" s="48"/>
+      <c r="D259" s="49"/>
+      <c r="E259" s="38"/>
+      <c r="F259" s="39"/>
+      <c r="G259" s="38"/>
+      <c r="H259" s="39"/>
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A260" s="27" t="s">
+      <c r="A260" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="B260" s="28"/>
-      <c r="C260" s="103" t="s">
+      <c r="B260" s="30"/>
+      <c r="C260" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="D260" s="104"/>
-      <c r="E260" s="27"/>
-      <c r="F260" s="28"/>
-      <c r="G260" s="27"/>
-      <c r="H260" s="28"/>
+      <c r="D260" s="51"/>
+      <c r="E260" s="29"/>
+      <c r="F260" s="30"/>
+      <c r="G260" s="29"/>
+      <c r="H260" s="30"/>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A261" s="29"/>
-      <c r="B261" s="30"/>
-      <c r="C261" s="105"/>
-      <c r="D261" s="106"/>
-      <c r="E261" s="29"/>
-      <c r="F261" s="30"/>
-      <c r="G261" s="29"/>
-      <c r="H261" s="30"/>
+      <c r="A261" s="31"/>
+      <c r="B261" s="32"/>
+      <c r="C261" s="52"/>
+      <c r="D261" s="53"/>
+      <c r="E261" s="31"/>
+      <c r="F261" s="32"/>
+      <c r="G261" s="31"/>
+      <c r="H261" s="32"/>
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A262" s="39" t="s">
+      <c r="A262" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="B262" s="40"/>
-      <c r="C262" s="99" t="s">
+      <c r="B262" s="37"/>
+      <c r="C262" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="D262" s="100"/>
-      <c r="E262" s="39"/>
-      <c r="F262" s="40"/>
-      <c r="G262" s="39"/>
-      <c r="H262" s="40"/>
+      <c r="D262" s="43"/>
+      <c r="E262" s="36"/>
+      <c r="F262" s="37"/>
+      <c r="G262" s="36"/>
+      <c r="H262" s="37"/>
       <c r="J262" s="2"/>
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A263" s="41"/>
-      <c r="B263" s="42"/>
-      <c r="C263" s="101"/>
-      <c r="D263" s="102"/>
-      <c r="E263" s="41"/>
-      <c r="F263" s="42"/>
-      <c r="G263" s="41"/>
-      <c r="H263" s="42"/>
+      <c r="A263" s="38"/>
+      <c r="B263" s="39"/>
+      <c r="C263" s="44"/>
+      <c r="D263" s="45"/>
+      <c r="E263" s="38"/>
+      <c r="F263" s="39"/>
+      <c r="G263" s="38"/>
+      <c r="H263" s="39"/>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A264" s="27" t="s">
+      <c r="A264" s="29" t="s">
         <v>255</v>
       </c>
-      <c r="B264" s="28"/>
-      <c r="C264" s="27" t="s">
+      <c r="B264" s="30"/>
+      <c r="C264" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="D264" s="28"/>
-      <c r="E264" s="27"/>
-      <c r="F264" s="28"/>
-      <c r="G264" s="27"/>
-      <c r="H264" s="28"/>
+      <c r="D264" s="30"/>
+      <c r="E264" s="29"/>
+      <c r="F264" s="30"/>
+      <c r="G264" s="29"/>
+      <c r="H264" s="30"/>
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A265" s="29"/>
-      <c r="B265" s="30"/>
-      <c r="C265" s="29"/>
-      <c r="D265" s="30"/>
-      <c r="E265" s="29"/>
-      <c r="F265" s="30"/>
-      <c r="G265" s="29"/>
-      <c r="H265" s="30"/>
+      <c r="A265" s="31"/>
+      <c r="B265" s="32"/>
+      <c r="C265" s="31"/>
+      <c r="D265" s="32"/>
+      <c r="E265" s="31"/>
+      <c r="F265" s="32"/>
+      <c r="G265" s="31"/>
+      <c r="H265" s="32"/>
     </row>
     <row r="273" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G273" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="519">
-    <mergeCell ref="E172:F173"/>
-    <mergeCell ref="G172:H173"/>
-    <mergeCell ref="E174:F175"/>
-    <mergeCell ref="G174:H175"/>
-    <mergeCell ref="E176:F177"/>
-    <mergeCell ref="G176:H177"/>
-    <mergeCell ref="E166:F167"/>
-    <mergeCell ref="G166:H167"/>
-    <mergeCell ref="E168:F169"/>
-    <mergeCell ref="G168:H169"/>
-    <mergeCell ref="E170:F171"/>
-    <mergeCell ref="G170:H171"/>
-    <mergeCell ref="E160:F161"/>
-    <mergeCell ref="G160:H161"/>
-    <mergeCell ref="E162:F163"/>
-    <mergeCell ref="G162:H163"/>
-    <mergeCell ref="E164:F165"/>
-    <mergeCell ref="G164:H165"/>
-    <mergeCell ref="E154:F155"/>
-    <mergeCell ref="G154:H155"/>
-    <mergeCell ref="E156:F157"/>
-    <mergeCell ref="G156:H157"/>
-    <mergeCell ref="E158:F159"/>
-    <mergeCell ref="G158:H159"/>
-    <mergeCell ref="E148:F149"/>
-    <mergeCell ref="G148:H149"/>
-    <mergeCell ref="E150:F151"/>
-    <mergeCell ref="G150:H151"/>
-    <mergeCell ref="E152:F153"/>
-    <mergeCell ref="G152:H153"/>
-    <mergeCell ref="E142:F143"/>
-    <mergeCell ref="G142:H143"/>
-    <mergeCell ref="E144:F145"/>
-    <mergeCell ref="G144:H145"/>
-    <mergeCell ref="E146:F147"/>
-    <mergeCell ref="G146:H147"/>
-    <mergeCell ref="E136:F137"/>
-    <mergeCell ref="G136:H137"/>
-    <mergeCell ref="E138:F139"/>
-    <mergeCell ref="G138:H139"/>
-    <mergeCell ref="E140:F141"/>
-    <mergeCell ref="G140:H141"/>
-    <mergeCell ref="E130:F131"/>
-    <mergeCell ref="G130:H131"/>
-    <mergeCell ref="E132:F133"/>
-    <mergeCell ref="G132:H133"/>
-    <mergeCell ref="E134:F135"/>
-    <mergeCell ref="G134:H135"/>
-    <mergeCell ref="E124:F125"/>
-    <mergeCell ref="G124:H125"/>
-    <mergeCell ref="E126:F127"/>
-    <mergeCell ref="G126:H127"/>
-    <mergeCell ref="E128:F129"/>
-    <mergeCell ref="G128:H129"/>
-    <mergeCell ref="E118:F119"/>
-    <mergeCell ref="G118:H119"/>
-    <mergeCell ref="E120:F121"/>
-    <mergeCell ref="G120:H121"/>
-    <mergeCell ref="E122:F123"/>
-    <mergeCell ref="G122:H123"/>
-    <mergeCell ref="E112:F113"/>
-    <mergeCell ref="G112:H113"/>
-    <mergeCell ref="E114:F115"/>
-    <mergeCell ref="G114:H115"/>
-    <mergeCell ref="E116:F117"/>
-    <mergeCell ref="G116:H117"/>
-    <mergeCell ref="E106:F107"/>
-    <mergeCell ref="G106:H107"/>
-    <mergeCell ref="E108:F109"/>
-    <mergeCell ref="G108:H109"/>
-    <mergeCell ref="E110:F111"/>
-    <mergeCell ref="G110:H111"/>
-    <mergeCell ref="E100:F101"/>
-    <mergeCell ref="G100:H101"/>
-    <mergeCell ref="E102:F103"/>
-    <mergeCell ref="G102:H103"/>
-    <mergeCell ref="E104:F105"/>
-    <mergeCell ref="G104:H105"/>
-    <mergeCell ref="E86:F87"/>
-    <mergeCell ref="G86:H87"/>
-    <mergeCell ref="E90:F91"/>
-    <mergeCell ref="G90:H91"/>
-    <mergeCell ref="E82:F83"/>
-    <mergeCell ref="G80:H81"/>
-    <mergeCell ref="G82:H83"/>
-    <mergeCell ref="E84:F85"/>
-    <mergeCell ref="G84:H85"/>
-    <mergeCell ref="E76:F77"/>
-    <mergeCell ref="G76:H77"/>
-    <mergeCell ref="E78:F79"/>
-    <mergeCell ref="G78:H79"/>
-    <mergeCell ref="E80:F81"/>
-    <mergeCell ref="G70:H71"/>
-    <mergeCell ref="E72:F73"/>
-    <mergeCell ref="G72:H73"/>
-    <mergeCell ref="E74:F75"/>
-    <mergeCell ref="G74:H75"/>
-    <mergeCell ref="E188:F189"/>
-    <mergeCell ref="A184:H185"/>
-    <mergeCell ref="E186:F187"/>
-    <mergeCell ref="G186:H187"/>
-    <mergeCell ref="G188:H189"/>
-    <mergeCell ref="A178:B179"/>
-    <mergeCell ref="C178:D179"/>
-    <mergeCell ref="A180:B181"/>
-    <mergeCell ref="C180:D181"/>
-    <mergeCell ref="A182:B183"/>
-    <mergeCell ref="C182:D183"/>
-    <mergeCell ref="E178:F179"/>
-    <mergeCell ref="G178:H179"/>
-    <mergeCell ref="E180:F181"/>
-    <mergeCell ref="G180:H181"/>
-    <mergeCell ref="E182:F183"/>
-    <mergeCell ref="G182:H183"/>
-    <mergeCell ref="G206:H207"/>
-    <mergeCell ref="G208:H209"/>
-    <mergeCell ref="G190:H191"/>
-    <mergeCell ref="G192:H193"/>
-    <mergeCell ref="G194:H195"/>
-    <mergeCell ref="G196:H197"/>
-    <mergeCell ref="G198:H199"/>
-    <mergeCell ref="E196:F197"/>
-    <mergeCell ref="E194:F195"/>
-    <mergeCell ref="E192:F193"/>
-    <mergeCell ref="E190:F191"/>
-    <mergeCell ref="E206:F207"/>
-    <mergeCell ref="E204:F205"/>
-    <mergeCell ref="E202:F203"/>
-    <mergeCell ref="E200:F201"/>
-    <mergeCell ref="E198:F199"/>
-    <mergeCell ref="G200:H201"/>
-    <mergeCell ref="G202:H203"/>
-    <mergeCell ref="G204:H205"/>
-    <mergeCell ref="E212:F213"/>
-    <mergeCell ref="G214:H215"/>
-    <mergeCell ref="G212:H213"/>
-    <mergeCell ref="E210:F211"/>
-    <mergeCell ref="E208:F209"/>
-    <mergeCell ref="G210:H211"/>
-    <mergeCell ref="E218:F219"/>
-    <mergeCell ref="G218:H219"/>
-    <mergeCell ref="E216:F217"/>
-    <mergeCell ref="G216:H217"/>
-    <mergeCell ref="E214:F215"/>
-    <mergeCell ref="E224:F225"/>
-    <mergeCell ref="G224:H225"/>
-    <mergeCell ref="E222:F223"/>
-    <mergeCell ref="G222:H223"/>
-    <mergeCell ref="E220:F221"/>
-    <mergeCell ref="G220:H221"/>
-    <mergeCell ref="E228:F229"/>
-    <mergeCell ref="G228:H229"/>
-    <mergeCell ref="G230:H231"/>
-    <mergeCell ref="E226:F227"/>
-    <mergeCell ref="G226:H227"/>
-    <mergeCell ref="E234:F235"/>
-    <mergeCell ref="G234:H235"/>
-    <mergeCell ref="E232:F233"/>
-    <mergeCell ref="G232:H233"/>
-    <mergeCell ref="E230:F231"/>
-    <mergeCell ref="E240:F241"/>
-    <mergeCell ref="G240:H241"/>
-    <mergeCell ref="E238:F239"/>
-    <mergeCell ref="G238:H239"/>
-    <mergeCell ref="E236:F237"/>
-    <mergeCell ref="G236:H237"/>
-    <mergeCell ref="E248:F249"/>
-    <mergeCell ref="G248:H249"/>
-    <mergeCell ref="E246:F247"/>
-    <mergeCell ref="E242:F243"/>
-    <mergeCell ref="E244:F245"/>
-    <mergeCell ref="G242:H243"/>
-    <mergeCell ref="G244:H245"/>
-    <mergeCell ref="G246:H247"/>
-    <mergeCell ref="E254:F255"/>
-    <mergeCell ref="G254:H255"/>
-    <mergeCell ref="E252:F253"/>
-    <mergeCell ref="G252:H253"/>
-    <mergeCell ref="E250:F251"/>
-    <mergeCell ref="G250:H251"/>
-    <mergeCell ref="E258:F259"/>
-    <mergeCell ref="G260:H261"/>
-    <mergeCell ref="G258:H259"/>
-    <mergeCell ref="E256:F257"/>
-    <mergeCell ref="G256:H257"/>
-    <mergeCell ref="E264:F265"/>
-    <mergeCell ref="G264:H265"/>
-    <mergeCell ref="E262:F263"/>
-    <mergeCell ref="G262:H263"/>
-    <mergeCell ref="E260:F261"/>
-    <mergeCell ref="A262:B263"/>
-    <mergeCell ref="C262:D263"/>
-    <mergeCell ref="A264:B265"/>
-    <mergeCell ref="C264:D265"/>
-    <mergeCell ref="A256:B257"/>
-    <mergeCell ref="C256:D257"/>
-    <mergeCell ref="A258:B259"/>
-    <mergeCell ref="C258:D259"/>
-    <mergeCell ref="A260:B261"/>
-    <mergeCell ref="C260:D261"/>
-    <mergeCell ref="A250:B251"/>
-    <mergeCell ref="C250:D251"/>
-    <mergeCell ref="A252:B253"/>
-    <mergeCell ref="C252:D253"/>
-    <mergeCell ref="A254:B255"/>
-    <mergeCell ref="C254:D255"/>
-    <mergeCell ref="A244:B245"/>
-    <mergeCell ref="C244:D245"/>
-    <mergeCell ref="A246:B247"/>
-    <mergeCell ref="C246:D247"/>
-    <mergeCell ref="A248:B249"/>
-    <mergeCell ref="C248:D249"/>
-    <mergeCell ref="A238:B239"/>
-    <mergeCell ref="C238:D239"/>
-    <mergeCell ref="A240:B241"/>
-    <mergeCell ref="C240:D241"/>
-    <mergeCell ref="A242:B243"/>
-    <mergeCell ref="C242:D243"/>
-    <mergeCell ref="A232:B233"/>
-    <mergeCell ref="C232:D233"/>
-    <mergeCell ref="A234:B235"/>
-    <mergeCell ref="C234:D235"/>
-    <mergeCell ref="A236:B237"/>
-    <mergeCell ref="C236:D237"/>
-    <mergeCell ref="A226:B227"/>
-    <mergeCell ref="C226:D227"/>
-    <mergeCell ref="A228:B229"/>
-    <mergeCell ref="C228:D229"/>
-    <mergeCell ref="A230:B231"/>
-    <mergeCell ref="C230:D231"/>
-    <mergeCell ref="A220:B221"/>
-    <mergeCell ref="C220:D221"/>
-    <mergeCell ref="A222:B223"/>
-    <mergeCell ref="C222:D223"/>
-    <mergeCell ref="A224:B225"/>
-    <mergeCell ref="C224:D225"/>
-    <mergeCell ref="A214:B215"/>
-    <mergeCell ref="C214:D215"/>
-    <mergeCell ref="A216:B217"/>
-    <mergeCell ref="C216:D217"/>
-    <mergeCell ref="A218:B219"/>
-    <mergeCell ref="C218:D219"/>
-    <mergeCell ref="A208:B209"/>
-    <mergeCell ref="C208:D209"/>
-    <mergeCell ref="A210:B211"/>
-    <mergeCell ref="C210:D211"/>
-    <mergeCell ref="A212:B213"/>
-    <mergeCell ref="C212:D213"/>
-    <mergeCell ref="A202:B203"/>
-    <mergeCell ref="C202:D203"/>
-    <mergeCell ref="A204:B205"/>
-    <mergeCell ref="C204:D205"/>
-    <mergeCell ref="A206:B207"/>
-    <mergeCell ref="C206:D207"/>
-    <mergeCell ref="A196:B197"/>
-    <mergeCell ref="C196:D197"/>
-    <mergeCell ref="A198:B199"/>
-    <mergeCell ref="C198:D199"/>
-    <mergeCell ref="A200:B201"/>
-    <mergeCell ref="C200:D201"/>
-    <mergeCell ref="A190:B191"/>
-    <mergeCell ref="C190:D191"/>
-    <mergeCell ref="A192:B193"/>
-    <mergeCell ref="C192:D193"/>
-    <mergeCell ref="A194:B195"/>
-    <mergeCell ref="C194:D195"/>
-    <mergeCell ref="A186:B187"/>
-    <mergeCell ref="C186:D187"/>
-    <mergeCell ref="A188:B189"/>
-    <mergeCell ref="C188:D189"/>
-    <mergeCell ref="A176:B177"/>
-    <mergeCell ref="C176:D177"/>
-    <mergeCell ref="A166:B167"/>
-    <mergeCell ref="C166:D167"/>
-    <mergeCell ref="A168:B169"/>
-    <mergeCell ref="C168:D169"/>
-    <mergeCell ref="A170:B171"/>
-    <mergeCell ref="C170:D171"/>
-    <mergeCell ref="A160:B161"/>
-    <mergeCell ref="C160:D161"/>
-    <mergeCell ref="A162:B163"/>
-    <mergeCell ref="C162:D163"/>
-    <mergeCell ref="A164:B165"/>
-    <mergeCell ref="C164:D165"/>
-    <mergeCell ref="A172:B173"/>
-    <mergeCell ref="C172:D173"/>
-    <mergeCell ref="A174:B175"/>
-    <mergeCell ref="C174:D175"/>
-    <mergeCell ref="A154:B155"/>
-    <mergeCell ref="C154:D155"/>
-    <mergeCell ref="A156:B157"/>
-    <mergeCell ref="C156:D157"/>
-    <mergeCell ref="A158:B159"/>
-    <mergeCell ref="C158:D159"/>
-    <mergeCell ref="A148:B149"/>
-    <mergeCell ref="C148:D149"/>
-    <mergeCell ref="A150:B151"/>
-    <mergeCell ref="C150:D151"/>
-    <mergeCell ref="A152:B153"/>
-    <mergeCell ref="C152:D153"/>
-    <mergeCell ref="A142:B143"/>
-    <mergeCell ref="C142:D143"/>
-    <mergeCell ref="A144:B145"/>
-    <mergeCell ref="C144:D145"/>
-    <mergeCell ref="A146:B147"/>
-    <mergeCell ref="C146:D147"/>
-    <mergeCell ref="A136:B137"/>
-    <mergeCell ref="C136:D137"/>
-    <mergeCell ref="A138:B139"/>
-    <mergeCell ref="C138:D139"/>
-    <mergeCell ref="A140:B141"/>
-    <mergeCell ref="C140:D141"/>
-    <mergeCell ref="A130:B131"/>
-    <mergeCell ref="C130:D131"/>
-    <mergeCell ref="A132:B133"/>
-    <mergeCell ref="C132:D133"/>
-    <mergeCell ref="A134:B135"/>
-    <mergeCell ref="C134:D135"/>
-    <mergeCell ref="A124:B125"/>
-    <mergeCell ref="C124:D125"/>
-    <mergeCell ref="A126:B127"/>
-    <mergeCell ref="C126:D127"/>
-    <mergeCell ref="A128:B129"/>
-    <mergeCell ref="C128:D129"/>
-    <mergeCell ref="A118:B119"/>
-    <mergeCell ref="C118:D119"/>
-    <mergeCell ref="A120:B121"/>
-    <mergeCell ref="C120:D121"/>
-    <mergeCell ref="A122:B123"/>
-    <mergeCell ref="C122:D123"/>
-    <mergeCell ref="A112:B113"/>
-    <mergeCell ref="C112:D113"/>
-    <mergeCell ref="A114:B115"/>
-    <mergeCell ref="C114:D115"/>
-    <mergeCell ref="A116:B117"/>
-    <mergeCell ref="C116:D117"/>
-    <mergeCell ref="A106:B107"/>
-    <mergeCell ref="C106:D107"/>
-    <mergeCell ref="A108:B109"/>
-    <mergeCell ref="C108:D109"/>
-    <mergeCell ref="A110:B111"/>
-    <mergeCell ref="C110:D111"/>
-    <mergeCell ref="A100:B101"/>
-    <mergeCell ref="C100:D101"/>
-    <mergeCell ref="A102:B103"/>
-    <mergeCell ref="C102:D103"/>
-    <mergeCell ref="A104:B105"/>
-    <mergeCell ref="C104:D105"/>
-    <mergeCell ref="A96:B97"/>
-    <mergeCell ref="C96:D97"/>
-    <mergeCell ref="A98:B99"/>
-    <mergeCell ref="C98:D99"/>
-    <mergeCell ref="A88:H89"/>
-    <mergeCell ref="E94:F95"/>
-    <mergeCell ref="G94:H95"/>
-    <mergeCell ref="E96:F97"/>
-    <mergeCell ref="G96:H97"/>
-    <mergeCell ref="E98:F99"/>
-    <mergeCell ref="G98:H99"/>
-    <mergeCell ref="A90:B91"/>
-    <mergeCell ref="C92:D93"/>
-    <mergeCell ref="A94:B95"/>
-    <mergeCell ref="C94:D95"/>
-    <mergeCell ref="E92:F93"/>
-    <mergeCell ref="G92:H93"/>
-    <mergeCell ref="A86:B87"/>
-    <mergeCell ref="C86:D87"/>
-    <mergeCell ref="A92:B93"/>
-    <mergeCell ref="C90:D91"/>
-    <mergeCell ref="A74:B75"/>
-    <mergeCell ref="C74:D75"/>
-    <mergeCell ref="A78:B79"/>
-    <mergeCell ref="C78:D79"/>
-    <mergeCell ref="A82:B83"/>
-    <mergeCell ref="C82:D83"/>
-    <mergeCell ref="A84:B85"/>
-    <mergeCell ref="C84:D85"/>
-    <mergeCell ref="A76:B77"/>
-    <mergeCell ref="C76:D77"/>
-    <mergeCell ref="A80:B81"/>
-    <mergeCell ref="C80:D81"/>
-    <mergeCell ref="A70:B71"/>
-    <mergeCell ref="C70:D71"/>
-    <mergeCell ref="A72:B73"/>
-    <mergeCell ref="C72:D73"/>
-    <mergeCell ref="A64:B65"/>
-    <mergeCell ref="C64:D65"/>
-    <mergeCell ref="E54:F55"/>
-    <mergeCell ref="E64:F65"/>
-    <mergeCell ref="E66:F67"/>
-    <mergeCell ref="E68:F69"/>
-    <mergeCell ref="E70:F71"/>
-    <mergeCell ref="A66:B67"/>
-    <mergeCell ref="C66:D67"/>
-    <mergeCell ref="A60:B61"/>
-    <mergeCell ref="C60:D61"/>
-    <mergeCell ref="G58:H59"/>
-    <mergeCell ref="E60:F61"/>
-    <mergeCell ref="G60:H61"/>
-    <mergeCell ref="E62:F63"/>
-    <mergeCell ref="G62:H63"/>
-    <mergeCell ref="A54:B55"/>
-    <mergeCell ref="C54:D55"/>
-    <mergeCell ref="A68:B69"/>
-    <mergeCell ref="C68:D69"/>
-    <mergeCell ref="G68:H69"/>
-    <mergeCell ref="G64:H65"/>
-    <mergeCell ref="E40:F41"/>
-    <mergeCell ref="G40:H41"/>
-    <mergeCell ref="A46:B47"/>
-    <mergeCell ref="C46:D47"/>
-    <mergeCell ref="A48:B49"/>
-    <mergeCell ref="C48:D49"/>
-    <mergeCell ref="G66:H67"/>
-    <mergeCell ref="A62:B63"/>
-    <mergeCell ref="C62:D63"/>
-    <mergeCell ref="E52:F53"/>
-    <mergeCell ref="G52:H53"/>
-    <mergeCell ref="A58:B59"/>
-    <mergeCell ref="C58:D59"/>
-    <mergeCell ref="E46:F47"/>
-    <mergeCell ref="G46:H47"/>
-    <mergeCell ref="E48:F49"/>
-    <mergeCell ref="G48:H49"/>
-    <mergeCell ref="G54:H55"/>
-    <mergeCell ref="A56:B57"/>
-    <mergeCell ref="C56:D57"/>
-    <mergeCell ref="E56:F57"/>
-    <mergeCell ref="G56:H57"/>
-    <mergeCell ref="E58:F59"/>
+    <mergeCell ref="A1:H3"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="G6:H7"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="G16:H17"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="G14:H15"/>
+    <mergeCell ref="E20:F21"/>
+    <mergeCell ref="G20:H21"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="E4:F5"/>
+    <mergeCell ref="G4:H5"/>
+    <mergeCell ref="A28:B29"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="A8:B9"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="G8:H9"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="E10:F11"/>
+    <mergeCell ref="E12:F13"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="G10:H11"/>
+    <mergeCell ref="G12:H13"/>
+    <mergeCell ref="G18:H19"/>
+    <mergeCell ref="G22:H23"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E34:F35"/>
+    <mergeCell ref="G32:H33"/>
+    <mergeCell ref="G34:H35"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="A26:B27"/>
+    <mergeCell ref="C16:D17"/>
+    <mergeCell ref="E38:F39"/>
+    <mergeCell ref="G38:H39"/>
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="E28:F29"/>
+    <mergeCell ref="G28:H29"/>
+    <mergeCell ref="A34:B35"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="C26:D27"/>
+    <mergeCell ref="E36:F37"/>
+    <mergeCell ref="G36:H37"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="E24:F25"/>
+    <mergeCell ref="G24:H25"/>
     <mergeCell ref="E26:F27"/>
     <mergeCell ref="G26:H27"/>
     <mergeCell ref="A32:B33"/>
@@ -5371,71 +5014,436 @@
     <mergeCell ref="C30:D31"/>
     <mergeCell ref="E44:F45"/>
     <mergeCell ref="G44:H45"/>
-    <mergeCell ref="E34:F35"/>
-    <mergeCell ref="G32:H33"/>
-    <mergeCell ref="G34:H35"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="A26:B27"/>
-    <mergeCell ref="C16:D17"/>
-    <mergeCell ref="E38:F39"/>
-    <mergeCell ref="G38:H39"/>
-    <mergeCell ref="A38:B39"/>
-    <mergeCell ref="C38:D39"/>
-    <mergeCell ref="E28:F29"/>
-    <mergeCell ref="G28:H29"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="C26:D27"/>
-    <mergeCell ref="E36:F37"/>
-    <mergeCell ref="G36:H37"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="E24:F25"/>
-    <mergeCell ref="G24:H25"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="C28:D29"/>
-    <mergeCell ref="A8:B9"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="E8:F9"/>
-    <mergeCell ref="G8:H9"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="E10:F11"/>
-    <mergeCell ref="E12:F13"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="G10:H11"/>
-    <mergeCell ref="G12:H13"/>
-    <mergeCell ref="G18:H19"/>
-    <mergeCell ref="G22:H23"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="G14:H15"/>
-    <mergeCell ref="E20:F21"/>
-    <mergeCell ref="G20:H21"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="C4:D5"/>
-    <mergeCell ref="E4:F5"/>
-    <mergeCell ref="G4:H5"/>
-    <mergeCell ref="A1:H3"/>
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="G6:H7"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="G16:H17"/>
-    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="E40:F41"/>
+    <mergeCell ref="G40:H41"/>
+    <mergeCell ref="A46:B47"/>
+    <mergeCell ref="C46:D47"/>
+    <mergeCell ref="A48:B49"/>
+    <mergeCell ref="C48:D49"/>
+    <mergeCell ref="G66:H67"/>
+    <mergeCell ref="A62:B63"/>
+    <mergeCell ref="C62:D63"/>
+    <mergeCell ref="E52:F53"/>
+    <mergeCell ref="G52:H53"/>
+    <mergeCell ref="A58:B59"/>
+    <mergeCell ref="C58:D59"/>
+    <mergeCell ref="E46:F47"/>
+    <mergeCell ref="G46:H47"/>
+    <mergeCell ref="E48:F49"/>
+    <mergeCell ref="G48:H49"/>
+    <mergeCell ref="G54:H55"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="C56:D57"/>
+    <mergeCell ref="E56:F57"/>
+    <mergeCell ref="G56:H57"/>
+    <mergeCell ref="E58:F59"/>
+    <mergeCell ref="G58:H59"/>
+    <mergeCell ref="E60:F61"/>
+    <mergeCell ref="G60:H61"/>
+    <mergeCell ref="E62:F63"/>
+    <mergeCell ref="G62:H63"/>
+    <mergeCell ref="A54:B55"/>
+    <mergeCell ref="C54:D55"/>
+    <mergeCell ref="A68:B69"/>
+    <mergeCell ref="C68:D69"/>
+    <mergeCell ref="G68:H69"/>
+    <mergeCell ref="G64:H65"/>
+    <mergeCell ref="A70:B71"/>
+    <mergeCell ref="C70:D71"/>
+    <mergeCell ref="A72:B73"/>
+    <mergeCell ref="C72:D73"/>
+    <mergeCell ref="A64:B65"/>
+    <mergeCell ref="C64:D65"/>
+    <mergeCell ref="E54:F55"/>
+    <mergeCell ref="E64:F65"/>
+    <mergeCell ref="E66:F67"/>
+    <mergeCell ref="E68:F69"/>
+    <mergeCell ref="E70:F71"/>
+    <mergeCell ref="A66:B67"/>
+    <mergeCell ref="C66:D67"/>
+    <mergeCell ref="A60:B61"/>
+    <mergeCell ref="C60:D61"/>
+    <mergeCell ref="C86:D87"/>
+    <mergeCell ref="A92:B93"/>
+    <mergeCell ref="C90:D91"/>
+    <mergeCell ref="A74:B75"/>
+    <mergeCell ref="C74:D75"/>
+    <mergeCell ref="A78:B79"/>
+    <mergeCell ref="C78:D79"/>
+    <mergeCell ref="A82:B83"/>
+    <mergeCell ref="C82:D83"/>
+    <mergeCell ref="A84:B85"/>
+    <mergeCell ref="C84:D85"/>
+    <mergeCell ref="A76:B77"/>
+    <mergeCell ref="C76:D77"/>
+    <mergeCell ref="A80:B81"/>
+    <mergeCell ref="C80:D81"/>
+    <mergeCell ref="A100:B101"/>
+    <mergeCell ref="C100:D101"/>
+    <mergeCell ref="A102:B103"/>
+    <mergeCell ref="C102:D103"/>
+    <mergeCell ref="A104:B105"/>
+    <mergeCell ref="C104:D105"/>
+    <mergeCell ref="A96:B97"/>
+    <mergeCell ref="C96:D97"/>
+    <mergeCell ref="A98:B99"/>
+    <mergeCell ref="C98:D99"/>
+    <mergeCell ref="A112:B113"/>
+    <mergeCell ref="C112:D113"/>
+    <mergeCell ref="A114:B115"/>
+    <mergeCell ref="C114:D115"/>
+    <mergeCell ref="A116:B117"/>
+    <mergeCell ref="C116:D117"/>
+    <mergeCell ref="A106:B107"/>
+    <mergeCell ref="C106:D107"/>
+    <mergeCell ref="A108:B109"/>
+    <mergeCell ref="C108:D109"/>
+    <mergeCell ref="A110:B111"/>
+    <mergeCell ref="C110:D111"/>
+    <mergeCell ref="A124:B125"/>
+    <mergeCell ref="C124:D125"/>
+    <mergeCell ref="A126:B127"/>
+    <mergeCell ref="C126:D127"/>
+    <mergeCell ref="A128:B129"/>
+    <mergeCell ref="C128:D129"/>
+    <mergeCell ref="A118:B119"/>
+    <mergeCell ref="C118:D119"/>
+    <mergeCell ref="A120:B121"/>
+    <mergeCell ref="C120:D121"/>
+    <mergeCell ref="A122:B123"/>
+    <mergeCell ref="C122:D123"/>
+    <mergeCell ref="A136:B137"/>
+    <mergeCell ref="C136:D137"/>
+    <mergeCell ref="A138:B139"/>
+    <mergeCell ref="C138:D139"/>
+    <mergeCell ref="A140:B141"/>
+    <mergeCell ref="C140:D141"/>
+    <mergeCell ref="A130:B131"/>
+    <mergeCell ref="C130:D131"/>
+    <mergeCell ref="A132:B133"/>
+    <mergeCell ref="C132:D133"/>
+    <mergeCell ref="A134:B135"/>
+    <mergeCell ref="C134:D135"/>
+    <mergeCell ref="A148:B149"/>
+    <mergeCell ref="C148:D149"/>
+    <mergeCell ref="A150:B151"/>
+    <mergeCell ref="C150:D151"/>
+    <mergeCell ref="A152:B153"/>
+    <mergeCell ref="C152:D153"/>
+    <mergeCell ref="A142:B143"/>
+    <mergeCell ref="C142:D143"/>
+    <mergeCell ref="A144:B145"/>
+    <mergeCell ref="C144:D145"/>
+    <mergeCell ref="A146:B147"/>
+    <mergeCell ref="C146:D147"/>
+    <mergeCell ref="A172:B173"/>
+    <mergeCell ref="C172:D173"/>
+    <mergeCell ref="A174:B175"/>
+    <mergeCell ref="C174:D175"/>
+    <mergeCell ref="A154:B155"/>
+    <mergeCell ref="C154:D155"/>
+    <mergeCell ref="A156:B157"/>
+    <mergeCell ref="C156:D157"/>
+    <mergeCell ref="A158:B159"/>
+    <mergeCell ref="C158:D159"/>
+    <mergeCell ref="A166:B167"/>
+    <mergeCell ref="C166:D167"/>
+    <mergeCell ref="A168:B169"/>
+    <mergeCell ref="C168:D169"/>
+    <mergeCell ref="A170:B171"/>
+    <mergeCell ref="C170:D171"/>
+    <mergeCell ref="A160:B161"/>
+    <mergeCell ref="C160:D161"/>
+    <mergeCell ref="A162:B163"/>
+    <mergeCell ref="C162:D163"/>
+    <mergeCell ref="A164:B165"/>
+    <mergeCell ref="C164:D165"/>
+    <mergeCell ref="A190:B191"/>
+    <mergeCell ref="C190:D191"/>
+    <mergeCell ref="A192:B193"/>
+    <mergeCell ref="C192:D193"/>
+    <mergeCell ref="A194:B195"/>
+    <mergeCell ref="C194:D195"/>
+    <mergeCell ref="A186:B187"/>
+    <mergeCell ref="C186:D187"/>
+    <mergeCell ref="A188:B189"/>
+    <mergeCell ref="C188:D189"/>
+    <mergeCell ref="A202:B203"/>
+    <mergeCell ref="C202:D203"/>
+    <mergeCell ref="A204:B205"/>
+    <mergeCell ref="C204:D205"/>
+    <mergeCell ref="A206:B207"/>
+    <mergeCell ref="C206:D207"/>
+    <mergeCell ref="A196:B197"/>
+    <mergeCell ref="C196:D197"/>
+    <mergeCell ref="A198:B199"/>
+    <mergeCell ref="C198:D199"/>
+    <mergeCell ref="A200:B201"/>
+    <mergeCell ref="C200:D201"/>
+    <mergeCell ref="A214:B215"/>
+    <mergeCell ref="C214:D215"/>
+    <mergeCell ref="A216:B217"/>
+    <mergeCell ref="C216:D217"/>
+    <mergeCell ref="A218:B219"/>
+    <mergeCell ref="C218:D219"/>
+    <mergeCell ref="A208:B209"/>
+    <mergeCell ref="C208:D209"/>
+    <mergeCell ref="A210:B211"/>
+    <mergeCell ref="C210:D211"/>
+    <mergeCell ref="A212:B213"/>
+    <mergeCell ref="C212:D213"/>
+    <mergeCell ref="A226:B227"/>
+    <mergeCell ref="C226:D227"/>
+    <mergeCell ref="A228:B229"/>
+    <mergeCell ref="C228:D229"/>
+    <mergeCell ref="A230:B231"/>
+    <mergeCell ref="C230:D231"/>
+    <mergeCell ref="A220:B221"/>
+    <mergeCell ref="C220:D221"/>
+    <mergeCell ref="A222:B223"/>
+    <mergeCell ref="C222:D223"/>
+    <mergeCell ref="A224:B225"/>
+    <mergeCell ref="C224:D225"/>
+    <mergeCell ref="A238:B239"/>
+    <mergeCell ref="C238:D239"/>
+    <mergeCell ref="A240:B241"/>
+    <mergeCell ref="C240:D241"/>
+    <mergeCell ref="A242:B243"/>
+    <mergeCell ref="C242:D243"/>
+    <mergeCell ref="A232:B233"/>
+    <mergeCell ref="C232:D233"/>
+    <mergeCell ref="A234:B235"/>
+    <mergeCell ref="C234:D235"/>
+    <mergeCell ref="A236:B237"/>
+    <mergeCell ref="C236:D237"/>
+    <mergeCell ref="A250:B251"/>
+    <mergeCell ref="C250:D251"/>
+    <mergeCell ref="A252:B253"/>
+    <mergeCell ref="C252:D253"/>
+    <mergeCell ref="A254:B255"/>
+    <mergeCell ref="C254:D255"/>
+    <mergeCell ref="A244:B245"/>
+    <mergeCell ref="C244:D245"/>
+    <mergeCell ref="A246:B247"/>
+    <mergeCell ref="C246:D247"/>
+    <mergeCell ref="A248:B249"/>
+    <mergeCell ref="C248:D249"/>
+    <mergeCell ref="A262:B263"/>
+    <mergeCell ref="C262:D263"/>
+    <mergeCell ref="A264:B265"/>
+    <mergeCell ref="C264:D265"/>
+    <mergeCell ref="A256:B257"/>
+    <mergeCell ref="C256:D257"/>
+    <mergeCell ref="A258:B259"/>
+    <mergeCell ref="C258:D259"/>
+    <mergeCell ref="A260:B261"/>
+    <mergeCell ref="C260:D261"/>
+    <mergeCell ref="E258:F259"/>
+    <mergeCell ref="G260:H261"/>
+    <mergeCell ref="G258:H259"/>
+    <mergeCell ref="E256:F257"/>
+    <mergeCell ref="G256:H257"/>
+    <mergeCell ref="E264:F265"/>
+    <mergeCell ref="G264:H265"/>
+    <mergeCell ref="E262:F263"/>
+    <mergeCell ref="G262:H263"/>
+    <mergeCell ref="E260:F261"/>
+    <mergeCell ref="E248:F249"/>
+    <mergeCell ref="G248:H249"/>
+    <mergeCell ref="E246:F247"/>
+    <mergeCell ref="E242:F243"/>
+    <mergeCell ref="E244:F245"/>
+    <mergeCell ref="G242:H243"/>
+    <mergeCell ref="G244:H245"/>
+    <mergeCell ref="G246:H247"/>
+    <mergeCell ref="E254:F255"/>
+    <mergeCell ref="G254:H255"/>
+    <mergeCell ref="E252:F253"/>
+    <mergeCell ref="G252:H253"/>
+    <mergeCell ref="E250:F251"/>
+    <mergeCell ref="G250:H251"/>
+    <mergeCell ref="E234:F235"/>
+    <mergeCell ref="G234:H235"/>
+    <mergeCell ref="E232:F233"/>
+    <mergeCell ref="G232:H233"/>
+    <mergeCell ref="E230:F231"/>
+    <mergeCell ref="E240:F241"/>
+    <mergeCell ref="G240:H241"/>
+    <mergeCell ref="E238:F239"/>
+    <mergeCell ref="G238:H239"/>
+    <mergeCell ref="E236:F237"/>
+    <mergeCell ref="G236:H237"/>
+    <mergeCell ref="E224:F225"/>
+    <mergeCell ref="G224:H225"/>
+    <mergeCell ref="E222:F223"/>
+    <mergeCell ref="G222:H223"/>
+    <mergeCell ref="E220:F221"/>
+    <mergeCell ref="G220:H221"/>
+    <mergeCell ref="E228:F229"/>
+    <mergeCell ref="G228:H229"/>
+    <mergeCell ref="G230:H231"/>
+    <mergeCell ref="E226:F227"/>
+    <mergeCell ref="G226:H227"/>
+    <mergeCell ref="E212:F213"/>
+    <mergeCell ref="G214:H215"/>
+    <mergeCell ref="G212:H213"/>
+    <mergeCell ref="E210:F211"/>
+    <mergeCell ref="E208:F209"/>
+    <mergeCell ref="G210:H211"/>
+    <mergeCell ref="E218:F219"/>
+    <mergeCell ref="G218:H219"/>
+    <mergeCell ref="E216:F217"/>
+    <mergeCell ref="G216:H217"/>
+    <mergeCell ref="E214:F215"/>
+    <mergeCell ref="G206:H207"/>
+    <mergeCell ref="G208:H209"/>
+    <mergeCell ref="G190:H191"/>
+    <mergeCell ref="G192:H193"/>
+    <mergeCell ref="G194:H195"/>
+    <mergeCell ref="G196:H197"/>
+    <mergeCell ref="G198:H199"/>
+    <mergeCell ref="E196:F197"/>
+    <mergeCell ref="E194:F195"/>
+    <mergeCell ref="E192:F193"/>
+    <mergeCell ref="E190:F191"/>
+    <mergeCell ref="E206:F207"/>
+    <mergeCell ref="E204:F205"/>
+    <mergeCell ref="E202:F203"/>
+    <mergeCell ref="E200:F201"/>
+    <mergeCell ref="E198:F199"/>
+    <mergeCell ref="G200:H201"/>
+    <mergeCell ref="G202:H203"/>
+    <mergeCell ref="G204:H205"/>
+    <mergeCell ref="G70:H71"/>
+    <mergeCell ref="E72:F73"/>
+    <mergeCell ref="G72:H73"/>
+    <mergeCell ref="E74:F75"/>
+    <mergeCell ref="G74:H75"/>
+    <mergeCell ref="E188:F189"/>
+    <mergeCell ref="A184:H185"/>
+    <mergeCell ref="E186:F187"/>
+    <mergeCell ref="G186:H187"/>
+    <mergeCell ref="G188:H189"/>
+    <mergeCell ref="A178:B179"/>
+    <mergeCell ref="C178:D179"/>
+    <mergeCell ref="A180:B181"/>
+    <mergeCell ref="C180:D181"/>
+    <mergeCell ref="A182:B183"/>
+    <mergeCell ref="C182:D183"/>
+    <mergeCell ref="E178:F179"/>
+    <mergeCell ref="G178:H179"/>
+    <mergeCell ref="E180:F181"/>
+    <mergeCell ref="G180:H181"/>
+    <mergeCell ref="E182:F183"/>
+    <mergeCell ref="G182:H183"/>
+    <mergeCell ref="A176:B177"/>
+    <mergeCell ref="C176:D177"/>
+    <mergeCell ref="E82:F83"/>
+    <mergeCell ref="G80:H81"/>
+    <mergeCell ref="G82:H83"/>
+    <mergeCell ref="E84:F85"/>
+    <mergeCell ref="G84:H85"/>
+    <mergeCell ref="E76:F77"/>
+    <mergeCell ref="G76:H77"/>
+    <mergeCell ref="E78:F79"/>
+    <mergeCell ref="G78:H79"/>
+    <mergeCell ref="E80:F81"/>
+    <mergeCell ref="E100:F101"/>
+    <mergeCell ref="G100:H101"/>
+    <mergeCell ref="E102:F103"/>
+    <mergeCell ref="G102:H103"/>
+    <mergeCell ref="E104:F105"/>
+    <mergeCell ref="G104:H105"/>
+    <mergeCell ref="E86:F87"/>
+    <mergeCell ref="G86:H87"/>
+    <mergeCell ref="E90:F91"/>
+    <mergeCell ref="G90:H91"/>
+    <mergeCell ref="A88:H89"/>
+    <mergeCell ref="E94:F95"/>
+    <mergeCell ref="G94:H95"/>
+    <mergeCell ref="E96:F97"/>
+    <mergeCell ref="G96:H97"/>
+    <mergeCell ref="E98:F99"/>
+    <mergeCell ref="G98:H99"/>
+    <mergeCell ref="A90:B91"/>
+    <mergeCell ref="C92:D93"/>
+    <mergeCell ref="A94:B95"/>
+    <mergeCell ref="C94:D95"/>
+    <mergeCell ref="E92:F93"/>
+    <mergeCell ref="G92:H93"/>
+    <mergeCell ref="A86:B87"/>
+    <mergeCell ref="E112:F113"/>
+    <mergeCell ref="G112:H113"/>
+    <mergeCell ref="E114:F115"/>
+    <mergeCell ref="G114:H115"/>
+    <mergeCell ref="E116:F117"/>
+    <mergeCell ref="G116:H117"/>
+    <mergeCell ref="E106:F107"/>
+    <mergeCell ref="G106:H107"/>
+    <mergeCell ref="E108:F109"/>
+    <mergeCell ref="G108:H109"/>
+    <mergeCell ref="E110:F111"/>
+    <mergeCell ref="G110:H111"/>
+    <mergeCell ref="E124:F125"/>
+    <mergeCell ref="G124:H125"/>
+    <mergeCell ref="E126:F127"/>
+    <mergeCell ref="G126:H127"/>
+    <mergeCell ref="E128:F129"/>
+    <mergeCell ref="G128:H129"/>
+    <mergeCell ref="E118:F119"/>
+    <mergeCell ref="G118:H119"/>
+    <mergeCell ref="E120:F121"/>
+    <mergeCell ref="G120:H121"/>
+    <mergeCell ref="E122:F123"/>
+    <mergeCell ref="G122:H123"/>
+    <mergeCell ref="E136:F137"/>
+    <mergeCell ref="G136:H137"/>
+    <mergeCell ref="E138:F139"/>
+    <mergeCell ref="G138:H139"/>
+    <mergeCell ref="E140:F141"/>
+    <mergeCell ref="G140:H141"/>
+    <mergeCell ref="E130:F131"/>
+    <mergeCell ref="G130:H131"/>
+    <mergeCell ref="E132:F133"/>
+    <mergeCell ref="G132:H133"/>
+    <mergeCell ref="E134:F135"/>
+    <mergeCell ref="G134:H135"/>
+    <mergeCell ref="E148:F149"/>
+    <mergeCell ref="G148:H149"/>
+    <mergeCell ref="E150:F151"/>
+    <mergeCell ref="G150:H151"/>
+    <mergeCell ref="E152:F153"/>
+    <mergeCell ref="G152:H153"/>
+    <mergeCell ref="E142:F143"/>
+    <mergeCell ref="G142:H143"/>
+    <mergeCell ref="E144:F145"/>
+    <mergeCell ref="G144:H145"/>
+    <mergeCell ref="E146:F147"/>
+    <mergeCell ref="G146:H147"/>
+    <mergeCell ref="E160:F161"/>
+    <mergeCell ref="G160:H161"/>
+    <mergeCell ref="E162:F163"/>
+    <mergeCell ref="G162:H163"/>
+    <mergeCell ref="E164:F165"/>
+    <mergeCell ref="G164:H165"/>
+    <mergeCell ref="E154:F155"/>
+    <mergeCell ref="G154:H155"/>
+    <mergeCell ref="E156:F157"/>
+    <mergeCell ref="G156:H157"/>
+    <mergeCell ref="E158:F159"/>
+    <mergeCell ref="G158:H159"/>
+    <mergeCell ref="E172:F173"/>
+    <mergeCell ref="G172:H173"/>
+    <mergeCell ref="E174:F175"/>
+    <mergeCell ref="G174:H175"/>
+    <mergeCell ref="E176:F177"/>
+    <mergeCell ref="G176:H177"/>
+    <mergeCell ref="E166:F167"/>
+    <mergeCell ref="G166:H167"/>
+    <mergeCell ref="E168:F169"/>
+    <mergeCell ref="G168:H169"/>
+    <mergeCell ref="E170:F171"/>
+    <mergeCell ref="G170:H171"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Empezando integrador segunda entrega
</commit_message>
<xml_diff>
--- a/Documentacion/Proyecto/Tabla de Actividades/Tabla de actividades.xlsx
+++ b/Documentacion/Proyecto/Tabla de Actividades/Tabla de actividades.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\OneDrive\Trabajos\2020\Proyecto\Proyecto\Documentacion\Proyecto\Tabla de Actividades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="270">
   <si>
     <t>ByteSoft</t>
   </si>
@@ -822,6 +822,18 @@
   </si>
   <si>
     <t>Archivo crontab con backups</t>
+  </si>
+  <si>
+    <t>PROY03093, PROY03094</t>
+  </si>
+  <si>
+    <t>PROG03102, PROG03103</t>
+  </si>
+  <si>
+    <t>FEO3122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO03114, SO03115 </t>
   </si>
 </sst>
 </file>
@@ -1685,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C186" sqref="C186:D187"/>
+    <sheetView tabSelected="1" topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G208" sqref="G208:H209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -4332,9 +4344,13 @@
         <v>44</v>
       </c>
       <c r="D190" s="9"/>
-      <c r="E190" s="8"/>
+      <c r="E190" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="F190" s="9"/>
-      <c r="G190" s="8"/>
+      <c r="G190" s="8">
+        <v>1</v>
+      </c>
       <c r="H190" s="9"/>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
@@ -4356,9 +4372,13 @@
         <v>46</v>
       </c>
       <c r="D192" s="65"/>
-      <c r="E192" s="4"/>
+      <c r="E192" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="F192" s="5"/>
-      <c r="G192" s="4"/>
+      <c r="G192" s="4">
+        <v>1</v>
+      </c>
       <c r="H192" s="5"/>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
@@ -4380,9 +4400,13 @@
         <v>50</v>
       </c>
       <c r="D194" s="9"/>
-      <c r="E194" s="8"/>
+      <c r="E194" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="F194" s="9"/>
-      <c r="G194" s="8"/>
+      <c r="G194" s="8">
+        <v>1</v>
+      </c>
       <c r="H194" s="9"/>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
@@ -4404,9 +4428,13 @@
         <v>49</v>
       </c>
       <c r="D196" s="5"/>
-      <c r="E196" s="4"/>
+      <c r="E196" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="F196" s="5"/>
-      <c r="G196" s="4"/>
+      <c r="G196" s="4">
+        <v>1</v>
+      </c>
       <c r="H196" s="5"/>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
@@ -4428,9 +4456,13 @@
         <v>91</v>
       </c>
       <c r="D198" s="61"/>
-      <c r="E198" s="8"/>
+      <c r="E198" s="8" t="s">
+        <v>266</v>
+      </c>
       <c r="F198" s="9"/>
-      <c r="G198" s="8"/>
+      <c r="G198" s="8">
+        <v>2</v>
+      </c>
       <c r="H198" s="9"/>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
@@ -4452,9 +4484,13 @@
         <v>52</v>
       </c>
       <c r="D200" s="65"/>
-      <c r="E200" s="4"/>
+      <c r="E200" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="F200" s="5"/>
-      <c r="G200" s="4"/>
+      <c r="G200" s="4">
+        <v>3</v>
+      </c>
       <c r="H200" s="5"/>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
@@ -4476,9 +4512,13 @@
         <v>92</v>
       </c>
       <c r="D202" s="9"/>
-      <c r="E202" s="8"/>
+      <c r="E202" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="F202" s="9"/>
-      <c r="G202" s="8"/>
+      <c r="G202" s="8">
+        <v>3</v>
+      </c>
       <c r="H202" s="9"/>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
@@ -4500,9 +4540,13 @@
         <v>93</v>
       </c>
       <c r="D204" s="26"/>
-      <c r="E204" s="4"/>
+      <c r="E204" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="F204" s="5"/>
-      <c r="G204" s="4"/>
+      <c r="G204" s="4">
+        <v>2</v>
+      </c>
       <c r="H204" s="5"/>
       <c r="J204" s="2"/>
     </row>
@@ -4525,9 +4569,13 @@
         <v>94</v>
       </c>
       <c r="D206" s="61"/>
-      <c r="E206" s="8"/>
+      <c r="E206" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="F206" s="9"/>
-      <c r="G206" s="8"/>
+      <c r="G206" s="8">
+        <v>1</v>
+      </c>
       <c r="H206" s="9"/>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
@@ -4550,9 +4598,13 @@
         <v>95</v>
       </c>
       <c r="D208" s="5"/>
-      <c r="E208" s="4"/>
+      <c r="E208" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="F208" s="5"/>
-      <c r="G208" s="4"/>
+      <c r="G208" s="4">
+        <v>2</v>
+      </c>
       <c r="H208" s="5"/>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
@@ -4574,9 +4626,13 @@
         <v>96</v>
       </c>
       <c r="D210" s="61"/>
-      <c r="E210" s="8"/>
+      <c r="E210" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="F210" s="9"/>
-      <c r="G210" s="8"/>
+      <c r="G210" s="8">
+        <v>3</v>
+      </c>
       <c r="H210" s="9"/>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
@@ -4598,9 +4654,13 @@
         <v>97</v>
       </c>
       <c r="D212" s="5"/>
-      <c r="E212" s="4"/>
+      <c r="E212" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="F212" s="5"/>
-      <c r="G212" s="4"/>
+      <c r="G212" s="4">
+        <v>8</v>
+      </c>
       <c r="H212" s="5"/>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
@@ -4618,20 +4678,24 @@
         <v>144</v>
       </c>
       <c r="B214" s="9"/>
-      <c r="C214" s="8" t="s">
+      <c r="C214" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="D214" s="9"/>
-      <c r="E214" s="8"/>
+      <c r="D214" s="51"/>
+      <c r="E214" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="F214" s="9"/>
-      <c r="G214" s="8"/>
+      <c r="G214" s="8">
+        <v>3</v>
+      </c>
       <c r="H214" s="9"/>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="10"/>
       <c r="B215" s="11"/>
-      <c r="C215" s="10"/>
-      <c r="D215" s="11"/>
+      <c r="C215" s="52"/>
+      <c r="D215" s="53"/>
       <c r="E215" s="10"/>
       <c r="F215" s="11"/>
       <c r="G215" s="10"/>
@@ -4646,9 +4710,13 @@
         <v>98</v>
       </c>
       <c r="D216" s="26"/>
-      <c r="E216" s="4"/>
+      <c r="E216" s="4" t="s">
+        <v>267</v>
+      </c>
       <c r="F216" s="5"/>
-      <c r="G216" s="4"/>
+      <c r="G216" s="4">
+        <v>5</v>
+      </c>
       <c r="H216" s="5"/>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
@@ -4670,9 +4738,13 @@
         <v>99</v>
       </c>
       <c r="D218" s="9"/>
-      <c r="E218" s="8"/>
+      <c r="E218" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="F218" s="9"/>
-      <c r="G218" s="8"/>
+      <c r="G218" s="8">
+        <v>1</v>
+      </c>
       <c r="H218" s="9"/>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -4694,9 +4766,13 @@
         <v>100</v>
       </c>
       <c r="D220" s="5"/>
-      <c r="E220" s="4"/>
+      <c r="E220" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="F220" s="5"/>
-      <c r="G220" s="4"/>
+      <c r="G220" s="4">
+        <v>2</v>
+      </c>
       <c r="H220" s="5"/>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
@@ -4718,9 +4794,13 @@
         <v>101</v>
       </c>
       <c r="D222" s="9"/>
-      <c r="E222" s="8"/>
+      <c r="E222" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="F222" s="9"/>
-      <c r="G222" s="8"/>
+      <c r="G222" s="8">
+        <v>4</v>
+      </c>
       <c r="H222" s="9"/>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
@@ -4742,9 +4822,13 @@
         <v>102</v>
       </c>
       <c r="D224" s="5"/>
-      <c r="E224" s="4"/>
+      <c r="E224" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="F224" s="5"/>
-      <c r="G224" s="4"/>
+      <c r="G224" s="4">
+        <v>4</v>
+      </c>
       <c r="H224" s="5"/>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
@@ -4766,9 +4850,13 @@
         <v>103</v>
       </c>
       <c r="D226" s="9"/>
-      <c r="E226" s="8"/>
+      <c r="E226" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="F226" s="9"/>
-      <c r="G226" s="8"/>
+      <c r="G226" s="8">
+        <v>2</v>
+      </c>
       <c r="H226" s="9"/>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
@@ -4790,9 +4878,13 @@
         <v>104</v>
       </c>
       <c r="D228" s="5"/>
-      <c r="E228" s="4"/>
+      <c r="E228" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="F228" s="5"/>
-      <c r="G228" s="4"/>
+      <c r="G228" s="4">
+        <v>3</v>
+      </c>
       <c r="H228" s="5"/>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
@@ -4814,9 +4906,13 @@
         <v>105</v>
       </c>
       <c r="D230" s="51"/>
-      <c r="E230" s="8"/>
+      <c r="E230" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="F230" s="9"/>
-      <c r="G230" s="8"/>
+      <c r="G230" s="8">
+        <v>3</v>
+      </c>
       <c r="H230" s="9"/>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
@@ -4838,9 +4934,13 @@
         <v>106</v>
       </c>
       <c r="D232" s="59"/>
-      <c r="E232" s="16"/>
-      <c r="F232" s="17"/>
-      <c r="G232" s="16"/>
+      <c r="E232" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F232" s="5"/>
+      <c r="G232" s="16">
+        <v>3</v>
+      </c>
       <c r="H232" s="17"/>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
@@ -4862,9 +4962,13 @@
         <v>107</v>
       </c>
       <c r="D234" s="9"/>
-      <c r="E234" s="12"/>
+      <c r="E234" s="12" t="s">
+        <v>142</v>
+      </c>
       <c r="F234" s="9"/>
-      <c r="G234" s="8"/>
+      <c r="G234" s="8">
+        <v>5</v>
+      </c>
       <c r="H234" s="9"/>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
@@ -4886,9 +4990,13 @@
         <v>108</v>
       </c>
       <c r="D236" s="17"/>
-      <c r="E236" s="4"/>
+      <c r="E236" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="F236" s="5"/>
-      <c r="G236" s="4"/>
+      <c r="G236" s="4">
+        <v>3</v>
+      </c>
       <c r="H236" s="5"/>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.25">
@@ -4910,9 +5018,13 @@
         <v>109</v>
       </c>
       <c r="D238" s="9"/>
-      <c r="E238" s="8"/>
+      <c r="E238" s="8" t="s">
+        <v>132</v>
+      </c>
       <c r="F238" s="9"/>
-      <c r="G238" s="8"/>
+      <c r="G238" s="8">
+        <v>3</v>
+      </c>
       <c r="H238" s="9"/>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
@@ -4934,9 +5046,13 @@
         <v>110</v>
       </c>
       <c r="D240" s="5"/>
-      <c r="E240" s="4"/>
+      <c r="E240" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="F240" s="5"/>
-      <c r="G240" s="4"/>
+      <c r="G240" s="4">
+        <v>2</v>
+      </c>
       <c r="H240" s="5"/>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
@@ -4958,9 +5074,13 @@
         <v>111</v>
       </c>
       <c r="D242" s="30"/>
-      <c r="E242" s="29"/>
+      <c r="E242" s="29" t="s">
+        <v>132</v>
+      </c>
       <c r="F242" s="30"/>
-      <c r="G242" s="29"/>
+      <c r="G242" s="29">
+        <v>2</v>
+      </c>
       <c r="H242" s="30"/>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
@@ -4982,9 +5102,13 @@
         <v>112</v>
       </c>
       <c r="D244" s="26"/>
-      <c r="E244" s="4"/>
+      <c r="E244" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="F244" s="5"/>
-      <c r="G244" s="4"/>
+      <c r="G244" s="4">
+        <v>3</v>
+      </c>
       <c r="H244" s="5"/>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
@@ -5006,9 +5130,13 @@
         <v>113</v>
       </c>
       <c r="D246" s="9"/>
-      <c r="E246" s="8"/>
+      <c r="E246" s="8" t="s">
+        <v>269</v>
+      </c>
       <c r="F246" s="9"/>
-      <c r="G246" s="8"/>
+      <c r="G246" s="8">
+        <v>1</v>
+      </c>
       <c r="H246" s="9"/>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
@@ -5030,9 +5158,13 @@
         <v>114</v>
       </c>
       <c r="D248" s="26"/>
-      <c r="E248" s="4"/>
+      <c r="E248" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="F248" s="5"/>
-      <c r="G248" s="4"/>
+      <c r="G248" s="4">
+        <v>3</v>
+      </c>
       <c r="H248" s="5"/>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
@@ -5054,9 +5186,13 @@
         <v>115</v>
       </c>
       <c r="D250" s="51"/>
-      <c r="E250" s="8"/>
+      <c r="E250" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="F250" s="9"/>
-      <c r="G250" s="8"/>
+      <c r="G250" s="8">
+        <v>2</v>
+      </c>
       <c r="H250" s="9"/>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
@@ -5078,9 +5214,13 @@
         <v>116</v>
       </c>
       <c r="D252" s="5"/>
-      <c r="E252" s="33"/>
+      <c r="E252" s="33" t="s">
+        <v>136</v>
+      </c>
       <c r="F252" s="34"/>
-      <c r="G252" s="37"/>
+      <c r="G252" s="37">
+        <v>2</v>
+      </c>
       <c r="H252" s="38"/>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
@@ -5102,9 +5242,13 @@
         <v>117</v>
       </c>
       <c r="D254" s="15"/>
-      <c r="E254" s="44"/>
+      <c r="E254" s="44" t="s">
+        <v>268</v>
+      </c>
       <c r="F254" s="45"/>
-      <c r="G254" s="44"/>
+      <c r="G254" s="44">
+        <v>2</v>
+      </c>
       <c r="H254" s="45"/>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
@@ -5126,9 +5270,13 @@
         <v>118</v>
       </c>
       <c r="D256" s="5"/>
-      <c r="E256" s="33"/>
+      <c r="E256" s="33" t="s">
+        <v>136</v>
+      </c>
       <c r="F256" s="34"/>
-      <c r="G256" s="33"/>
+      <c r="G256" s="33">
+        <v>2</v>
+      </c>
       <c r="H256" s="34"/>
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.25">
@@ -5150,9 +5298,13 @@
         <v>119</v>
       </c>
       <c r="D258" s="9"/>
-      <c r="E258" s="40"/>
+      <c r="E258" s="40" t="s">
+        <v>139</v>
+      </c>
       <c r="F258" s="41"/>
-      <c r="G258" s="40"/>
+      <c r="G258" s="40">
+        <v>2</v>
+      </c>
       <c r="H258" s="41"/>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.25">
@@ -5174,9 +5326,13 @@
         <v>120</v>
       </c>
       <c r="D260" s="5"/>
-      <c r="E260" s="33"/>
+      <c r="E260" s="33" t="s">
+        <v>142</v>
+      </c>
       <c r="F260" s="34"/>
-      <c r="G260" s="33"/>
+      <c r="G260" s="33">
+        <v>1</v>
+      </c>
       <c r="H260" s="34"/>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.25">
@@ -5198,9 +5354,13 @@
         <v>121</v>
       </c>
       <c r="D262" s="51"/>
-      <c r="E262" s="40"/>
+      <c r="E262" s="40" t="s">
+        <v>142</v>
+      </c>
       <c r="F262" s="41"/>
-      <c r="G262" s="40"/>
+      <c r="G262" s="40">
+        <v>2</v>
+      </c>
       <c r="H262" s="41"/>
       <c r="J262" s="2"/>
     </row>
@@ -5223,9 +5383,13 @@
         <v>122</v>
       </c>
       <c r="D264" s="55"/>
-      <c r="E264" s="33"/>
+      <c r="E264" s="33" t="s">
+        <v>142</v>
+      </c>
       <c r="F264" s="34"/>
-      <c r="G264" s="33"/>
+      <c r="G264" s="33">
+        <v>4</v>
+      </c>
       <c r="H264" s="34"/>
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.25">
@@ -5247,9 +5411,13 @@
         <v>123</v>
       </c>
       <c r="D266" s="47"/>
-      <c r="E266" s="40"/>
+      <c r="E266" s="40" t="s">
+        <v>142</v>
+      </c>
       <c r="F266" s="41"/>
-      <c r="G266" s="40"/>
+      <c r="G266" s="40">
+        <v>3</v>
+      </c>
       <c r="H266" s="41"/>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.25">
@@ -5271,9 +5439,13 @@
         <v>124</v>
       </c>
       <c r="D268" s="34"/>
-      <c r="E268" s="33"/>
+      <c r="E268" s="33" t="s">
+        <v>142</v>
+      </c>
       <c r="F268" s="34"/>
-      <c r="G268" s="33"/>
+      <c r="G268" s="33">
+        <v>2</v>
+      </c>
       <c r="H268" s="34"/>
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>